<commit_message>
se agregaron variables artificales
</commit_message>
<xml_diff>
--- a/Datos/database.xlsx
+++ b/Datos/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1011" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1012" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1013" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1014" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1011" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="1012" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="1013" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="1014" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,15 +503,30 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>solido_dias</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>censura</t>
         </is>
@@ -522,16 +537,16 @@
         <v>43542</v>
       </c>
       <c r="B2" t="n">
-        <v>3567.266048919877</v>
+        <v>3650.530909409599</v>
       </c>
       <c r="C2" t="n">
-        <v>4439.0440133623</v>
+        <v>4412.927118283291</v>
       </c>
       <c r="D2" t="n">
-        <v>69.99898307790389</v>
+        <v>70.61407686496278</v>
       </c>
       <c r="E2" t="n">
-        <v>9.815360833056353</v>
+        <v>9.744629691280496</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -561,12 +576,21 @@
         <v>196</v>
       </c>
       <c r="M2" t="n">
+        <v>0.3584470906850903</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.02983850575991303</v>
+      </c>
+      <c r="O2" t="n">
+        <v>8.171472346277135e-06</v>
+      </c>
+      <c r="P2" t="n">
         <v>9.856424967447916</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -575,16 +599,16 @@
         <v>44694</v>
       </c>
       <c r="B3" t="n">
-        <v>3756.696993421127</v>
+        <v>3588.963390664635</v>
       </c>
       <c r="C3" t="n">
         <v>4076.248046875</v>
       </c>
       <c r="D3" t="n">
-        <v>71.44424529974734</v>
+        <v>71.04684454337131</v>
       </c>
       <c r="E3" t="n">
-        <v>9.866353379924323</v>
+        <v>9.854144088067248</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -614,12 +638,21 @@
         <v>697</v>
       </c>
       <c r="M3" t="n">
+        <v>0.1017863102340563</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.008041052003354516</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.239867687459316e-06</v>
+      </c>
+      <c r="P3" t="n">
         <v>37.43439031051377</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -667,12 +700,21 @@
         <v>18</v>
       </c>
       <c r="M4" t="n">
+        <v>3.135224392539576</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.3996208499708468</v>
+      </c>
+      <c r="O4" t="n">
+        <v>7.111241961163332e-05</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.6341090069593148</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -681,16 +723,16 @@
         <v>44694</v>
       </c>
       <c r="B5" t="n">
-        <v>3738.033099547425</v>
+        <v>3617.100425324863</v>
       </c>
       <c r="C5" t="n">
-        <v>4269.164080770409</v>
+        <v>4311.331527894737</v>
       </c>
       <c r="D5" t="n">
-        <v>71.36287906225283</v>
+        <v>69.97358904742886</v>
       </c>
       <c r="E5" t="n">
-        <v>9.806812164642452</v>
+        <v>9.820228855691296</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -720,12 +762,21 @@
         <v>948</v>
       </c>
       <c r="M5" t="n">
+        <v>0.07373402428601566</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.005236896399280996</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.447414939796939e-06</v>
+      </c>
+      <c r="P5" t="n">
         <v>56.13719472163866</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -734,16 +785,16 @@
         <v>44694</v>
       </c>
       <c r="B6" t="n">
-        <v>3738.033099547425</v>
+        <v>3617.100425324863</v>
       </c>
       <c r="C6" t="n">
-        <v>4269.164080770409</v>
+        <v>4311.331527894737</v>
       </c>
       <c r="D6" t="n">
-        <v>71.36287906225283</v>
+        <v>69.97358904742886</v>
       </c>
       <c r="E6" t="n">
-        <v>9.806812164642452</v>
+        <v>9.820228855691296</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -773,12 +824,21 @@
         <v>948</v>
       </c>
       <c r="M6" t="n">
+        <v>0.07373402428601566</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.01148095994725339</v>
+      </c>
+      <c r="O6" t="n">
+        <v>3.173195981856746e-06</v>
+      </c>
+      <c r="P6" t="n">
         <v>25.76638787493395</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -787,16 +847,16 @@
         <v>43046</v>
       </c>
       <c r="B7" t="n">
-        <v>3695.077720892984</v>
+        <v>3721.781582002402</v>
       </c>
       <c r="C7" t="n">
-        <v>4831.93534602042</v>
+        <v>4833.987603628011</v>
       </c>
       <c r="D7" t="n">
-        <v>70.4828642774178</v>
+        <v>70.23649846540003</v>
       </c>
       <c r="E7" t="n">
-        <v>9.793783350308377</v>
+        <v>9.770997781015527</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -826,12 +886,21 @@
         <v>56</v>
       </c>
       <c r="M7" t="n">
+        <v>1.232219271322808</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.0587259295298472</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.577462041430173e-05</v>
+      </c>
+      <c r="P7" t="n">
         <v>5.085127160904255</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -840,16 +909,16 @@
         <v>44694</v>
       </c>
       <c r="B8" t="n">
-        <v>3756.696993421127</v>
+        <v>3588.963390664635</v>
       </c>
       <c r="C8" t="n">
         <v>4076.248046875</v>
       </c>
       <c r="D8" t="n">
-        <v>71.44424529974734</v>
+        <v>71.04684454337131</v>
       </c>
       <c r="E8" t="n">
-        <v>9.866353379924323</v>
+        <v>9.854144088067248</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -879,12 +948,21 @@
         <v>697</v>
       </c>
       <c r="M8" t="n">
+        <v>0.1017863102340563</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.006566989132077147</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.829261864559514e-06</v>
+      </c>
+      <c r="P8" t="n">
         <v>45.07410481770833</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -893,16 +971,16 @@
         <v>43997</v>
       </c>
       <c r="B9" t="n">
-        <v>3741.034517047411</v>
+        <v>3653.801273259063</v>
       </c>
       <c r="C9" t="n">
-        <v>4083.616726624363</v>
+        <v>4146.867897310854</v>
       </c>
       <c r="D9" t="n">
-        <v>70.97058812462924</v>
+        <v>68.8866531023933</v>
       </c>
       <c r="E9" t="n">
-        <v>9.764257725265679</v>
+        <v>9.784382761838945</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -932,12 +1010,21 @@
         <v>251</v>
       </c>
       <c r="M9" t="n">
+        <v>0.2733597345333068</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.01837108501410016</v>
+      </c>
+      <c r="O9" t="n">
+        <v>5.026549316640296e-06</v>
+      </c>
+      <c r="P9" t="n">
         <v>15.61971842447917</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -946,13 +1033,13 @@
         <v>45545</v>
       </c>
       <c r="B10" t="n">
-        <v>4968.655946713799</v>
+        <v>5009.706697076511</v>
       </c>
       <c r="C10" t="n">
         <v>4812.063802083333</v>
       </c>
       <c r="D10" t="n">
-        <v>62.94341937514531</v>
+        <v>63.80976367292252</v>
       </c>
       <c r="E10" t="n">
         <v>7.701962391535442</v>
@@ -985,12 +1072,21 @@
         <v>41</v>
       </c>
       <c r="M10" t="n">
+        <v>1.519280087450536</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1364213702038822</v>
+      </c>
+      <c r="O10" t="n">
+        <v>2.722560336944977e-05</v>
+      </c>
+      <c r="P10" t="n">
         <v>2.007484879032258</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -999,16 +1095,16 @@
         <v>43542</v>
       </c>
       <c r="B11" t="n">
-        <v>3510.995510808461</v>
+        <v>3612.76202978949</v>
       </c>
       <c r="C11" t="n">
         <v>4612.53173828125</v>
       </c>
       <c r="D11" t="n">
-        <v>70.4642955957676</v>
+        <v>70.63041015624005</v>
       </c>
       <c r="E11" t="n">
-        <v>9.778685424959725</v>
+        <v>9.711176029157407</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1038,12 +1134,21 @@
         <v>70</v>
       </c>
       <c r="M11" t="n">
+        <v>0.9947945092428175</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1100411557696278</v>
+      </c>
+      <c r="O11" t="n">
+        <v>3.045011804539021e-05</v>
+      </c>
+      <c r="P11" t="n">
         <v>2.67022705078125</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1052,16 +1157,16 @@
         <v>44694</v>
       </c>
       <c r="B12" t="n">
-        <v>3738.033099547425</v>
+        <v>3617.100425324863</v>
       </c>
       <c r="C12" t="n">
-        <v>4269.164080770409</v>
+        <v>4311.331527894737</v>
       </c>
       <c r="D12" t="n">
-        <v>71.36287906225283</v>
+        <v>69.97358904742886</v>
       </c>
       <c r="E12" t="n">
-        <v>9.806812164642452</v>
+        <v>9.820228855691296</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1091,12 +1196,21 @@
         <v>948</v>
       </c>
       <c r="M12" t="n">
+        <v>0.07373402428601566</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.008466360505988289</v>
+      </c>
+      <c r="O12" t="n">
+        <v>2.339998785300527e-06</v>
+      </c>
+      <c r="P12" t="n">
         <v>34.43289998372396</v>
       </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1105,16 +1219,16 @@
         <v>45026</v>
       </c>
       <c r="B13" t="n">
-        <v>4066.808149855881</v>
+        <v>3976.10864418896</v>
       </c>
       <c r="C13" t="n">
-        <v>4260.239027374681</v>
+        <v>4291.864612717927</v>
       </c>
       <c r="D13" t="n">
-        <v>67.95560713451921</v>
+        <v>66.91363962340124</v>
       </c>
       <c r="E13" t="n">
-        <v>9.802506593956082</v>
+        <v>9.812569112242715</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1144,12 +1258,21 @@
         <v>1280</v>
       </c>
       <c r="M13" t="n">
+        <v>0.05223547199328746</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.003793981671296191</v>
+      </c>
+      <c r="O13" t="n">
+        <v>9.539542921960143e-07</v>
+      </c>
+      <c r="P13" t="n">
         <v>73.63584616388309</v>
       </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1158,16 +1281,16 @@
         <v>43375</v>
       </c>
       <c r="B14" t="n">
-        <v>3676.13869191971</v>
+        <v>3712.725517162844</v>
       </c>
       <c r="C14" t="n">
-        <v>4194.817015113633</v>
+        <v>4174.744402093462</v>
       </c>
       <c r="D14" t="n">
-        <v>71.68701402043241</v>
+        <v>72.01409690108343</v>
       </c>
       <c r="E14" t="n">
-        <v>9.734261293005442</v>
+        <v>9.695565910188543</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1197,12 +1320,21 @@
         <v>385</v>
       </c>
       <c r="M14" t="n">
+        <v>0.1865650178784545</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.01003800475267759</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2.702943752900525e-06</v>
+      </c>
+      <c r="P14" t="n">
         <v>29.88810221354167</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1250,12 +1382,21 @@
         <v>18</v>
       </c>
       <c r="M15" t="n">
+        <v>3.135224392539576</v>
+      </c>
+      <c r="N15" t="n">
+        <v>1.593659885600637</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.0002835612118066812</v>
+      </c>
+      <c r="P15" t="n">
         <v>0.1557983137044968</v>
       </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1270,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1341,15 +1482,30 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>solido_dias</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>censura</t>
         </is>
@@ -1360,16 +1516,16 @@
         <v>43164</v>
       </c>
       <c r="B2" t="n">
-        <v>4751.803722597938</v>
+        <v>4683.687231441381</v>
       </c>
       <c r="C2" t="n">
-        <v>4551.307888686591</v>
+        <v>4581.654082369169</v>
       </c>
       <c r="D2" t="n">
-        <v>71.71595578445806</v>
+        <v>71.48682329910575</v>
       </c>
       <c r="E2" t="n">
-        <v>10.07749458163147</v>
+        <v>10.0464199354169</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1399,12 +1555,21 @@
         <v>174</v>
       </c>
       <c r="M2" t="n">
+        <v>0.4084961331377471</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.02981427283291232</v>
+      </c>
+      <c r="O2" t="n">
+        <v>6.3641768358114e-06</v>
+      </c>
+      <c r="P2" t="n">
         <v>9.986409505208334</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1452,12 +1617,21 @@
         <v>70</v>
       </c>
       <c r="M3" t="n">
+        <v>0.927169853532818</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.06573200219134442</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1.317895359984026e-05</v>
+      </c>
+      <c r="P3" t="n">
         <v>4.257347074468085</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1466,16 +1640,16 @@
         <v>43828</v>
       </c>
       <c r="B4" t="n">
-        <v>5133.726074832364</v>
+        <v>5285.370327124099</v>
       </c>
       <c r="C4" t="n">
-        <v>4812.297113140109</v>
+        <v>4781.561368563385</v>
       </c>
       <c r="D4" t="n">
-        <v>68.90995381429789</v>
+        <v>68.79795605719015</v>
       </c>
       <c r="E4" t="n">
-        <v>9.873068364727832</v>
+        <v>9.900638094963512</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -1505,12 +1679,21 @@
         <v>82</v>
       </c>
       <c r="M4" t="n">
+        <v>0.8288910368336162</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.07041094427076795</v>
+      </c>
+      <c r="O4" t="n">
+        <v>1.331924761308067e-05</v>
+      </c>
+      <c r="P4" t="n">
         <v>4.067049153645834</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1525,7 +1708,7 @@
         <v>4754.181396484375</v>
       </c>
       <c r="D5" t="n">
-        <v>69.8820753640388</v>
+        <v>70.37839774737606</v>
       </c>
       <c r="E5" t="n">
         <v>9.813123226165771</v>
@@ -1558,12 +1741,21 @@
         <v>71</v>
       </c>
       <c r="M5" t="n">
+        <v>0.9774777464913341</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.06214888943312322</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.449720514238695e-05</v>
+      </c>
+      <c r="P5" t="n">
         <v>4.7142333984375</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1572,16 +1764,16 @@
         <v>43375</v>
       </c>
       <c r="B6" t="n">
-        <v>5160.841575514473</v>
+        <v>5068.179412333663</v>
       </c>
       <c r="C6" t="n">
-        <v>4512.089797786557</v>
+        <v>4484.841010636902</v>
       </c>
       <c r="D6" t="n">
         <v>78.40909576416016</v>
       </c>
       <c r="E6" t="n">
-        <v>9.824335865396826</v>
+        <v>9.82985390396753</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1611,12 +1803,21 @@
         <v>80</v>
       </c>
       <c r="M6" t="n">
+        <v>0.9680135279525945</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.06368428221159375</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1.256295684189824e-05</v>
+      </c>
+      <c r="P6" t="n">
         <v>5.125899251302084</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1664,12 +1865,21 @@
         <v>70</v>
       </c>
       <c r="M7" t="n">
+        <v>0.927169853532818</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.04884215070456671</v>
+      </c>
+      <c r="O7" t="n">
+        <v>9.792635341429095e-06</v>
+      </c>
+      <c r="P7" t="n">
         <v>5.61163330078125</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1678,16 +1888,16 @@
         <v>44135</v>
       </c>
       <c r="B8" t="n">
-        <v>4888.677932955383</v>
+        <v>4865.187917726187</v>
       </c>
       <c r="C8" t="n">
         <v>4539.75390625</v>
       </c>
       <c r="D8" t="n">
-        <v>68.25579455861958</v>
+        <v>68.58409301943999</v>
       </c>
       <c r="E8" t="n">
-        <v>9.862891449569968</v>
+        <v>9.904414102770033</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1717,12 +1927,21 @@
         <v>307</v>
       </c>
       <c r="M8" t="n">
+        <v>0.2226756266864935</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.01408101745102692</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2.893640220313794e-06</v>
+      </c>
+      <c r="P8" t="n">
         <v>20.29032236735025</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1770,12 +1989,21 @@
         <v>51</v>
       </c>
       <c r="M9" t="n">
+        <v>1.507867226233849</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.08963760657532198</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.681075481845689e-05</v>
+      </c>
+      <c r="P9" t="n">
         <v>3.640559895833333</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1823,12 +2051,21 @@
         <v>70</v>
       </c>
       <c r="M10" t="n">
+        <v>0.927169853532818</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.07241033915681093</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1.451791865756604e-05</v>
+      </c>
+      <c r="P10" t="n">
         <v>3.86430352393617</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1837,16 +2074,16 @@
         <v>43542</v>
       </c>
       <c r="B11" t="n">
-        <v>5226.10080077807</v>
+        <v>5179.769719187665</v>
       </c>
       <c r="C11" t="n">
-        <v>4256.739112760466</v>
+        <v>4243.114719185639</v>
       </c>
       <c r="D11" t="n">
         <v>74.21575037638347</v>
       </c>
       <c r="E11" t="n">
-        <v>9.690711722879891</v>
+        <v>9.693470742165244</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1876,12 +2113,21 @@
         <v>292</v>
       </c>
       <c r="M11" t="n">
+        <v>0.2532960763699095</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.02283738594681219</v>
+      </c>
+      <c r="O11" t="n">
+        <v>4.408097029976355e-06</v>
+      </c>
+      <c r="P11" t="n">
         <v>13.5364501953125</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1890,16 +2136,16 @@
         <v>44060</v>
       </c>
       <c r="B12" t="n">
-        <v>5067.563904096761</v>
+        <v>5036.243883791166</v>
       </c>
       <c r="C12" t="n">
         <v>4490.618815104167</v>
       </c>
       <c r="D12" t="n">
-        <v>68.64697270088081</v>
+        <v>69.08470398197467</v>
       </c>
       <c r="E12" t="n">
-        <v>9.80940089495885</v>
+        <v>9.864764432558937</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1929,12 +2175,21 @@
         <v>232</v>
       </c>
       <c r="M12" t="n">
+        <v>0.2965008754591187</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.02226476766022587</v>
+      </c>
+      <c r="O12" t="n">
+        <v>4.420019949112823e-06</v>
+      </c>
+      <c r="P12" t="n">
         <v>12.924462890625</v>
       </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1949,7 +2204,7 @@
         <v>4405.142415364583</v>
       </c>
       <c r="D13" t="n">
-        <v>69.74308912838806</v>
+        <v>70.45403724417395</v>
       </c>
       <c r="E13" t="n">
         <v>9.929780324300131</v>
@@ -1982,12 +2237,21 @@
         <v>110</v>
       </c>
       <c r="M13" t="n">
+        <v>0.6347210562538194</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.04197057033256762</v>
+      </c>
+      <c r="O13" t="n">
+        <v>9.473554196915129e-06</v>
+      </c>
+      <c r="P13" t="n">
         <v>7.18481079362955</v>
       </c>
-      <c r="N13" t="n">
-        <v>0</v>
-      </c>
-      <c r="O13" t="n">
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2002,7 +2266,7 @@
         <v>3991.271240234375</v>
       </c>
       <c r="D14" t="n">
-        <v>69.65556263046135</v>
+        <v>70.2592121459294</v>
       </c>
       <c r="E14" t="n">
         <v>9.812788645426433</v>
@@ -2035,12 +2299,21 @@
         <v>56</v>
       </c>
       <c r="M14" t="n">
+        <v>1.23261775694613</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.06805873499910294</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1.641905534198381e-05</v>
+      </c>
+      <c r="P14" t="n">
         <v>4.370050979872881</v>
       </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2049,16 +2322,16 @@
         <v>43164</v>
       </c>
       <c r="B15" t="n">
-        <v>4768.965201782987</v>
+        <v>4697.25159485301</v>
       </c>
       <c r="C15" t="n">
-        <v>4374.265543967385</v>
+        <v>4419.784834491255</v>
       </c>
       <c r="D15" t="n">
-        <v>74.13853938957772</v>
+        <v>73.79484066154924</v>
       </c>
       <c r="E15" t="n">
-        <v>9.804389894145199</v>
+        <v>9.757777924823355</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2088,12 +2361,21 @@
         <v>118</v>
       </c>
       <c r="M15" t="n">
+        <v>0.6201247114415903</v>
+      </c>
+      <c r="N15" t="n">
+        <v>44.19059464176984</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0.009361794461541669</v>
+      </c>
+      <c r="P15" t="n">
         <v>0.002850731382978723</v>
       </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2102,16 +2384,16 @@
         <v>43746</v>
       </c>
       <c r="B16" t="n">
-        <v>4965.227539676114</v>
+        <v>5116.871791967849</v>
       </c>
       <c r="C16" t="n">
-        <v>4678.029290874484</v>
+        <v>4647.29354629776</v>
       </c>
       <c r="D16" t="n">
-        <v>68.26691411092875</v>
+        <v>68.15491635382101</v>
       </c>
       <c r="E16" t="n">
-        <v>9.690688642132617</v>
+        <v>9.718258372368297</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -2141,12 +2423,21 @@
         <v>204</v>
       </c>
       <c r="M16" t="n">
+        <v>0.3324630066040049</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.0299580249544829</v>
+      </c>
+      <c r="O16" t="n">
+        <v>5.853592761066498e-06</v>
+      </c>
+      <c r="P16" t="n">
         <v>9.844215029761905</v>
       </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
+      <c r="Q16" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2161,7 +2452,7 @@
         <v>4655.380696614583</v>
       </c>
       <c r="D17" t="n">
-        <v>69.84850938785529</v>
+        <v>70.14927861099049</v>
       </c>
       <c r="E17" t="n">
         <v>9.917221069335938</v>
@@ -2194,12 +2485,21 @@
         <v>79</v>
       </c>
       <c r="M17" t="n">
+        <v>0.8768659826373811</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.2542047528260891</v>
+      </c>
+      <c r="O17" t="n">
+        <v>5.95363715268607e-05</v>
+      </c>
+      <c r="P17" t="n">
         <v>1.175024831396886</v>
       </c>
-      <c r="N17" t="n">
-        <v>0</v>
-      </c>
-      <c r="O17" t="n">
+      <c r="Q17" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2214,7 +2514,7 @@
         <v>4027.862711588542</v>
       </c>
       <c r="D18" t="n">
-        <v>69.56249129281996</v>
+        <v>70.37968260037316</v>
       </c>
       <c r="E18" t="n">
         <v>9.550990104675293</v>
@@ -2247,12 +2547,21 @@
         <v>42</v>
       </c>
       <c r="M18" t="n">
+        <v>1.636736804659841</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0.1805387067049497</v>
+      </c>
+      <c r="O18" t="n">
+        <v>4.119840263608161e-05</v>
+      </c>
+      <c r="P18" t="n">
         <v>1.66523144740364</v>
       </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
+      <c r="Q18" t="n">
+        <v>0</v>
+      </c>
+      <c r="R18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2261,16 +2570,16 @@
         <v>43046</v>
       </c>
       <c r="B19" t="n">
-        <v>4676.222257606293</v>
+        <v>4660.833787556601</v>
       </c>
       <c r="C19" t="n">
-        <v>4816.595744162698</v>
+        <v>4862.115034686567</v>
       </c>
       <c r="D19" t="n">
-        <v>68.36938579460701</v>
+        <v>68.02568706657854</v>
       </c>
       <c r="E19" t="n">
-        <v>10.21010267871429</v>
+        <v>10.2122063708624</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -2300,12 +2609,21 @@
         <v>56</v>
       </c>
       <c r="M19" t="n">
+        <v>1.193433106431202</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0.06790360646160216</v>
+      </c>
+      <c r="O19" t="n">
+        <v>1.456575138103923e-05</v>
+      </c>
+      <c r="P19" t="n">
         <v>4.169991048177083</v>
       </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
+      <c r="Q19" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2314,16 +2632,16 @@
         <v>43472</v>
       </c>
       <c r="B20" t="n">
-        <v>4765.051181631085</v>
+        <v>4626.05793685987</v>
       </c>
       <c r="C20" t="n">
-        <v>4662.602348047023</v>
+        <v>4621.72916732254</v>
       </c>
       <c r="D20" t="n">
         <v>72.18566513061523</v>
       </c>
       <c r="E20" t="n">
-        <v>9.799710947600854</v>
+        <v>9.807988005456911</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2353,12 +2671,21 @@
         <v>97</v>
       </c>
       <c r="M20" t="n">
+        <v>0.7365884197001554</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0.03476428682664822</v>
+      </c>
+      <c r="O20" t="n">
+        <v>7.513231237891394e-06</v>
+      </c>
+      <c r="P20" t="n">
         <v>8.647631835937499</v>
       </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
+      <c r="Q20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R20" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2373,7 +2700,7 @@
         <v>4378.823974609375</v>
       </c>
       <c r="D21" t="n">
-        <v>69.72394497483795</v>
+        <v>70.83553569715124</v>
       </c>
       <c r="E21" t="n">
         <v>9.831962108612061</v>
@@ -2406,12 +2733,21 @@
         <v>16</v>
       </c>
       <c r="M21" t="n">
+        <v>4.166796217479485</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.21561341959747</v>
+      </c>
+      <c r="O21" t="n">
+        <v>4.761763761051218e-05</v>
+      </c>
+      <c r="P21" t="n">
         <v>1.407219219924812</v>
       </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2420,16 +2756,16 @@
         <v>43164</v>
       </c>
       <c r="B22" t="n">
-        <v>4768.965201782987</v>
+        <v>4697.25159485301</v>
       </c>
       <c r="C22" t="n">
-        <v>4374.265543967385</v>
+        <v>4419.784834491255</v>
       </c>
       <c r="D22" t="n">
-        <v>74.13853938957772</v>
+        <v>73.79484066154924</v>
       </c>
       <c r="E22" t="n">
-        <v>9.804389894145199</v>
+        <v>9.757777924823355</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2459,12 +2795,21 @@
         <v>118</v>
       </c>
       <c r="M22" t="n">
+        <v>0.6201247114415903</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.03991411258924718</v>
+      </c>
+      <c r="O22" t="n">
+        <v>8.495488638426351e-06</v>
+      </c>
+      <c r="P22" t="n">
         <v>7.863152426861702</v>
       </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2473,16 +2818,16 @@
         <v>43375</v>
       </c>
       <c r="B23" t="n">
-        <v>5345.84285155773</v>
+        <v>5276.346229172123</v>
       </c>
       <c r="C23" t="n">
-        <v>4078.842800000074</v>
+        <v>4058.406209637832</v>
       </c>
       <c r="D23" t="n">
         <v>78.40909576416016</v>
       </c>
       <c r="E23" t="n">
-        <v>9.69357452706886</v>
+        <v>9.697713055996889</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2512,12 +2857,21 @@
         <v>125</v>
       </c>
       <c r="M23" t="n">
+        <v>0.6222944108266679</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0.0500094138348668</v>
+      </c>
+      <c r="O23" t="n">
+        <v>9.476197830123555e-06</v>
+      </c>
+      <c r="P23" t="n">
         <v>6.528694661458333</v>
       </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2526,16 +2880,16 @@
         <v>43828</v>
       </c>
       <c r="B24" t="n">
-        <v>5060.171387025557</v>
+        <v>5135.993513171425</v>
       </c>
       <c r="C24" t="n">
-        <v>4712.41442571068</v>
+        <v>4697.046553422318</v>
       </c>
       <c r="D24" t="n">
-        <v>67.36950670756399</v>
+        <v>67.31350782901012</v>
       </c>
       <c r="E24" t="n">
-        <v>9.779027239614893</v>
+        <v>9.792812104732732</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2565,12 +2919,21 @@
         <v>356</v>
       </c>
       <c r="M24" t="n">
+        <v>0.1885532432185157</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.01457808447601622</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2.837859100536628e-06</v>
+      </c>
+      <c r="P24" t="n">
         <v>19.23518880208333</v>
       </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2579,16 +2942,16 @@
         <v>45429</v>
       </c>
       <c r="B25" t="n">
-        <v>4479.992119873545</v>
+        <v>4493.997796344011</v>
       </c>
       <c r="C25" t="n">
         <v>4580.375390625</v>
       </c>
       <c r="D25" t="n">
-        <v>70.02925008507978</v>
+        <v>70.10875321602296</v>
       </c>
       <c r="E25" t="n">
-        <v>9.694824430447365</v>
+        <v>9.724858342718264</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2618,12 +2981,21 @@
         <v>230</v>
       </c>
       <c r="M25" t="n">
+        <v>0.3035010961732596</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.02371761257581382</v>
+      </c>
+      <c r="O25" t="n">
+        <v>5.276431953531767e-06</v>
+      </c>
+      <c r="P25" t="n">
         <v>12.44201480263158</v>
       </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2638,7 +3010,7 @@
         <v>3991.271240234375</v>
       </c>
       <c r="D26" t="n">
-        <v>69.65556263046135</v>
+        <v>70.2592121459294</v>
       </c>
       <c r="E26" t="n">
         <v>9.812788645426433</v>
@@ -2671,12 +3043,21 @@
         <v>56</v>
       </c>
       <c r="M26" t="n">
+        <v>1.23261775694613</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.1007461333678254</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2.430473938712802e-05</v>
+      </c>
+      <c r="P26" t="n">
         <v>2.963356050531915</v>
       </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2685,16 +3066,16 @@
         <v>43250</v>
       </c>
       <c r="B27" t="n">
-        <v>5039.064461870328</v>
+        <v>4987.977093502911</v>
       </c>
       <c r="C27" t="n">
-        <v>4108.256368175099</v>
+        <v>4131.016013437034</v>
       </c>
       <c r="D27" t="n">
-        <v>73.38924077938358</v>
+        <v>73.21739141536935</v>
       </c>
       <c r="E27" t="n">
-        <v>9.883443564244841</v>
+        <v>9.860137579583917</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2724,12 +3105,21 @@
         <v>260</v>
       </c>
       <c r="M27" t="n">
+        <v>0.280526403890304</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.01459763543538528</v>
+      </c>
+      <c r="O27" t="n">
+        <v>2.925973362006371e-06</v>
+      </c>
+      <c r="P27" t="n">
         <v>20.89459228515625</v>
       </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2738,16 +3128,16 @@
         <v>43472</v>
       </c>
       <c r="B28" t="n">
-        <v>5048.082353510855</v>
+        <v>4978.585731125248</v>
       </c>
       <c r="C28" t="n">
-        <v>4530.203334668043</v>
+        <v>4509.766744305802</v>
       </c>
       <c r="D28" t="n">
         <v>75.2973804473877</v>
       </c>
       <c r="E28" t="n">
-        <v>9.808950999542004</v>
+        <v>9.813089528470034</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2777,12 +3167,21 @@
         <v>177</v>
       </c>
       <c r="M28" t="n">
+        <v>0.423018991277459</v>
+      </c>
+      <c r="N28" t="n">
+        <v>0.03363710421051013</v>
+      </c>
+      <c r="O28" t="n">
+        <v>6.754977706567668e-06</v>
+      </c>
+      <c r="P28" t="n">
         <v>9.323006184895833</v>
       </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
+      <c r="Q28" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2791,16 +3190,16 @@
         <v>43746</v>
       </c>
       <c r="B29" t="n">
-        <v>4965.227539676114</v>
+        <v>5116.871791967849</v>
       </c>
       <c r="C29" t="n">
-        <v>4678.029290874484</v>
+        <v>4647.29354629776</v>
       </c>
       <c r="D29" t="n">
-        <v>68.26691411092875</v>
+        <v>68.15491635382101</v>
       </c>
       <c r="E29" t="n">
-        <v>9.690688642132617</v>
+        <v>9.718258372368297</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2830,12 +3229,21 @@
         <v>204</v>
       </c>
       <c r="M29" t="n">
+        <v>0.3324630066040049</v>
+      </c>
+      <c r="N29" t="n">
+        <v>0.03133691631485556</v>
+      </c>
+      <c r="O29" t="n">
+        <v>6.123017857908314e-06</v>
+      </c>
+      <c r="P29" t="n">
         <v>9.270397454690832</v>
       </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
+      <c r="Q29" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2850,7 +3258,7 @@
         <v>4754.181396484375</v>
       </c>
       <c r="D30" t="n">
-        <v>69.8820753640388</v>
+        <v>70.37839774737606</v>
       </c>
       <c r="E30" t="n">
         <v>9.813123226165771</v>
@@ -2883,12 +3291,21 @@
         <v>71</v>
       </c>
       <c r="M30" t="n">
+        <v>0.9774777464913341</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.08545088186131393</v>
+      </c>
+      <c r="O30" t="n">
+        <v>1.993270689932952e-05</v>
+      </c>
+      <c r="P30" t="n">
         <v>3.463630756578947</v>
       </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
+      <c r="Q30" t="n">
+        <v>0</v>
+      </c>
+      <c r="R30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2903,7 +3320,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2974,15 +3391,30 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>solido_dias</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>censura</t>
         </is>
@@ -2993,16 +3425,16 @@
         <v>43746</v>
       </c>
       <c r="B2" t="n">
-        <v>5206.332403115878</v>
+        <v>5178.888016214247</v>
       </c>
       <c r="C2" t="n">
-        <v>4719.457446778657</v>
+        <v>4656.25163973196</v>
       </c>
       <c r="D2" t="n">
         <v>76.89302062988281</v>
       </c>
       <c r="E2" t="n">
-        <v>9.921254725123225</v>
+        <v>9.910604755207157</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3032,12 +3464,21 @@
         <v>204</v>
       </c>
       <c r="M2" t="n">
+        <v>0.3750879055116235</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.02135445274105606</v>
+      </c>
+      <c r="O2" t="n">
+        <v>4.122561850124167e-06</v>
+      </c>
+      <c r="P2" t="n">
         <v>15.31827937998673</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3085,12 +3526,21 @@
         <v>62</v>
       </c>
       <c r="M3" t="n">
+        <v>1.244588821653336</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.09605830916150629</v>
+      </c>
+      <c r="O3" t="n">
+        <v>3.070943763881843e-05</v>
+      </c>
+      <c r="P3" t="n">
         <v>3.476612473347548</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3099,7 +3549,7 @@
         <v>43542</v>
       </c>
       <c r="B4" t="n">
-        <v>5201.946292841067</v>
+        <v>5080.875192379706</v>
       </c>
       <c r="C4" t="n">
         <v>4612.53173828125</v>
@@ -3108,7 +3558,7 @@
         <v>43.95745515823364</v>
       </c>
       <c r="E4" t="n">
-        <v>9.902906568215027</v>
+        <v>9.936217277876406</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -3138,12 +3588,21 @@
         <v>70</v>
       </c>
       <c r="M4" t="n">
+        <v>0.6191190867356851</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.04761618215460961</v>
+      </c>
+      <c r="O4" t="n">
+        <v>9.369761608907781e-06</v>
+      </c>
+      <c r="P4" t="n">
         <v>3.842342122395833</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3191,12 +3650,21 @@
         <v>62</v>
       </c>
       <c r="M5" t="n">
+        <v>1.244588821653336</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.08890747047063174</v>
+      </c>
+      <c r="O5" t="n">
+        <v>2.842337705823408e-05</v>
+      </c>
+      <c r="P5" t="n">
         <v>3.764606704059829</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3205,16 +3673,16 @@
         <v>43542</v>
       </c>
       <c r="B6" t="n">
-        <v>4997.984611338476</v>
+        <v>4892.269246478644</v>
       </c>
       <c r="C6" t="n">
-        <v>4656.362568166141</v>
+        <v>4671.947010454687</v>
       </c>
       <c r="D6" t="n">
-        <v>56.57983480961988</v>
+        <v>57.16271156068339</v>
       </c>
       <c r="E6" t="n">
-        <v>9.855278002107758</v>
+        <v>9.869223630887968</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -3244,12 +3712,21 @@
         <v>496</v>
       </c>
       <c r="M6" t="n">
+        <v>0.1150155162186789</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.01083914566161715</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.215110820739602e-06</v>
+      </c>
+      <c r="P6" t="n">
         <v>22.20096217105263</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3258,16 +3735,16 @@
         <v>43472</v>
       </c>
       <c r="B7" t="n">
-        <v>4831.624168008322</v>
+        <v>4634.52959909199</v>
       </c>
       <c r="C7" t="n">
-        <v>4670.351818791267</v>
+        <v>4657.780355045553</v>
       </c>
       <c r="D7" t="n">
-        <v>40.12388915350656</v>
+        <v>42.13005750213573</v>
       </c>
       <c r="E7" t="n">
-        <v>9.76144766601119</v>
+        <v>9.796923320138461</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -3297,12 +3774,21 @@
         <v>97</v>
       </c>
       <c r="M7" t="n">
+        <v>0.4298985459401605</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.04018553293483022</v>
+      </c>
+      <c r="O7" t="n">
+        <v>8.668989786833875e-06</v>
+      </c>
+      <c r="P7" t="n">
         <v>4.364119466145834</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3311,16 +3797,16 @@
         <v>43746</v>
       </c>
       <c r="B8" t="n">
-        <v>5206.332403115878</v>
+        <v>5178.888016214247</v>
       </c>
       <c r="C8" t="n">
-        <v>4719.457446778657</v>
+        <v>4656.25163973196</v>
       </c>
       <c r="D8" t="n">
         <v>76.89302062988281</v>
       </c>
       <c r="E8" t="n">
-        <v>9.921254725123225</v>
+        <v>9.910604755207157</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -3350,12 +3836,21 @@
         <v>204</v>
       </c>
       <c r="M8" t="n">
+        <v>0.3750879055116235</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.0217781871640179</v>
+      </c>
+      <c r="O8" t="n">
+        <v>4.204365290166943e-06</v>
+      </c>
+      <c r="P8" t="n">
         <v>14.9248862397595</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3364,16 +3859,16 @@
         <v>45549</v>
       </c>
       <c r="B9" t="n">
-        <v>3652.321318000452</v>
+        <v>3692.726455968947</v>
       </c>
       <c r="C9" t="n">
         <v>4623.30078125</v>
       </c>
       <c r="D9" t="n">
-        <v>74.39585989447708</v>
+        <v>74.49064665201698</v>
       </c>
       <c r="E9" t="n">
-        <v>10.28075615954284</v>
+        <v>10.26048695006634</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -3403,12 +3898,21 @@
         <v>45</v>
       </c>
       <c r="M9" t="n">
+        <v>1.619361883739499</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1589471557949093</v>
+      </c>
+      <c r="O9" t="n">
+        <v>4.303072734493526e-05</v>
+      </c>
+      <c r="P9" t="n">
         <v>2.007083221566524</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3417,16 +3921,16 @@
         <v>43542</v>
       </c>
       <c r="B10" t="n">
-        <v>5078.461033880548</v>
+        <v>4947.064654602994</v>
       </c>
       <c r="C10" t="n">
-        <v>4660.407722944178</v>
+        <v>4652.026747113702</v>
       </c>
       <c r="D10" t="n">
-        <v>51.87490793420619</v>
+        <v>53.21235349995897</v>
       </c>
       <c r="E10" t="n">
-        <v>9.85551690917673</v>
+        <v>9.879167345261578</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -3456,12 +3960,21 @@
         <v>167</v>
       </c>
       <c r="M10" t="n">
+        <v>0.3167401994045177</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.02210392641089216</v>
+      </c>
+      <c r="O10" t="n">
+        <v>4.467176276546567e-06</v>
+      </c>
+      <c r="P10" t="n">
         <v>10.02654622395833</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3470,16 +3983,16 @@
         <v>43472</v>
       </c>
       <c r="B11" t="n">
-        <v>4831.624168008322</v>
+        <v>4634.52959909199</v>
       </c>
       <c r="C11" t="n">
-        <v>4670.351818791267</v>
+        <v>4657.780355045553</v>
       </c>
       <c r="D11" t="n">
-        <v>40.12388915350656</v>
+        <v>42.13005750213573</v>
       </c>
       <c r="E11" t="n">
-        <v>9.76144766601119</v>
+        <v>9.796923320138461</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -3509,12 +4022,21 @@
         <v>97</v>
       </c>
       <c r="M11" t="n">
+        <v>0.4298985459401605</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.02318969386687898</v>
+      </c>
+      <c r="O11" t="n">
+        <v>5.002586083637527e-06</v>
+      </c>
+      <c r="P11" t="n">
         <v>7.726628989361702</v>
       </c>
-      <c r="N11" t="n">
-        <v>0</v>
-      </c>
-      <c r="O11" t="n">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3529,7 +4051,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3600,15 +4122,30 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
+          <t>solido_dias</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>censura</t>
         </is>
@@ -3619,16 +4156,16 @@
         <v>43472</v>
       </c>
       <c r="B2" t="n">
-        <v>5090.873982252704</v>
+        <v>5072.552669726541</v>
       </c>
       <c r="C2" t="n">
-        <v>4744.496128245028</v>
+        <v>4707.332692688629</v>
       </c>
       <c r="D2" t="n">
-        <v>70.52944989762824</v>
+        <v>70.83008186548328</v>
       </c>
       <c r="E2" t="n">
-        <v>9.935439978054765</v>
+        <v>9.945000384926107</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3658,12 +4195,21 @@
         <v>482</v>
       </c>
       <c r="M2" t="n">
+        <v>0.1466461322266735</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.01289458051285598</v>
+      </c>
+      <c r="O2" t="n">
+        <v>2.541525626382137e-06</v>
+      </c>
+      <c r="P2" t="n">
         <v>23.37026263297872</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3672,16 +4218,16 @@
         <v>43542</v>
       </c>
       <c r="B3" t="n">
-        <v>5058.290852369892</v>
+        <v>5039.969539843729</v>
       </c>
       <c r="C3" t="n">
-        <v>4678.277866526278</v>
+        <v>4641.114430969879</v>
       </c>
       <c r="D3" t="n">
-        <v>72.80084653459113</v>
+        <v>73.10147850244616</v>
       </c>
       <c r="E3" t="n">
-        <v>9.746337089947467</v>
+        <v>9.755897496818809</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -3711,12 +4257,21 @@
         <v>496</v>
       </c>
       <c r="M3" t="n">
+        <v>0.1470854698238353</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.01153703271950763</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2.288650908561155e-06</v>
+      </c>
+      <c r="P3" t="n">
         <v>26.39685872395833</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3725,16 +4280,16 @@
         <v>43472</v>
       </c>
       <c r="B4" t="n">
-        <v>5090.873982252704</v>
+        <v>5072.552669726541</v>
       </c>
       <c r="C4" t="n">
-        <v>4744.496128245028</v>
+        <v>4707.332692688629</v>
       </c>
       <c r="D4" t="n">
-        <v>70.52944989762824</v>
+        <v>70.83008186548328</v>
       </c>
       <c r="E4" t="n">
-        <v>9.935439978054765</v>
+        <v>9.945000384926107</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -3764,12 +4319,21 @@
         <v>482</v>
       </c>
       <c r="M4" t="n">
+        <v>0.1466461322266735</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0112224820716108</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2.211954894401083e-06</v>
+      </c>
+      <c r="P4" t="n">
         <v>26.85295877659575</v>
       </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3778,16 +4342,16 @@
         <v>45591</v>
       </c>
       <c r="B5" t="n">
-        <v>4945.517108443461</v>
+        <v>4938.916536289141</v>
       </c>
       <c r="C5" t="n">
-        <v>4583.328666845399</v>
+        <v>4591.316938915174</v>
       </c>
       <c r="D5" t="n">
-        <v>71.16876975999247</v>
+        <v>71.21276797447767</v>
       </c>
       <c r="E5" t="n">
-        <v>10.04189855144975</v>
+        <v>10.06287683723352</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -3817,12 +4381,21 @@
         <v>655</v>
       </c>
       <c r="M5" t="n">
+        <v>0.1085560487415818</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.007415551064993533</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.501147933289961e-06</v>
+      </c>
+      <c r="P5" t="n">
         <v>40.51546842035865</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3831,16 +4404,16 @@
         <v>43542</v>
       </c>
       <c r="B6" t="n">
-        <v>5058.290852369892</v>
+        <v>5039.969539843729</v>
       </c>
       <c r="C6" t="n">
-        <v>4678.277866526278</v>
+        <v>4641.114430969879</v>
       </c>
       <c r="D6" t="n">
-        <v>72.80084653459113</v>
+        <v>73.10147850244616</v>
       </c>
       <c r="E6" t="n">
-        <v>9.746337089947467</v>
+        <v>9.755897496818809</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -3870,12 +4443,21 @@
         <v>496</v>
       </c>
       <c r="M6" t="n">
+        <v>0.1470854698238353</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.0107054596514722</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2.123688349895906e-06</v>
+      </c>
+      <c r="P6" t="n">
         <v>28.44762369791667</v>
       </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3884,16 +4466,16 @@
         <v>45591</v>
       </c>
       <c r="B7" t="n">
-        <v>4945.517108443461</v>
+        <v>4938.916536289141</v>
       </c>
       <c r="C7" t="n">
-        <v>4583.328666845399</v>
+        <v>4591.316938915174</v>
       </c>
       <c r="D7" t="n">
-        <v>71.16876975999247</v>
+        <v>71.21276797447767</v>
       </c>
       <c r="E7" t="n">
-        <v>10.04189855144975</v>
+        <v>10.06287683723352</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -3923,12 +4505,21 @@
         <v>655</v>
       </c>
       <c r="M7" t="n">
+        <v>0.1085560487415818</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.007261284864460343</v>
+      </c>
+      <c r="O7" t="n">
+        <v>1.46991947624368e-06</v>
+      </c>
+      <c r="P7" t="n">
         <v>41.37631032436709</v>
       </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3937,16 +4528,16 @@
         <v>43746</v>
       </c>
       <c r="B8" t="n">
-        <v>5024.552795452553</v>
+        <v>4980.79850271789</v>
       </c>
       <c r="C8" t="n">
-        <v>4677.091021810086</v>
+        <v>4635.318122109912</v>
       </c>
       <c r="D8" t="n">
-        <v>72.17102419647041</v>
+        <v>72.48080129796253</v>
       </c>
       <c r="E8" t="n">
-        <v>9.753664850383412</v>
+        <v>9.758953231400747</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -3976,12 +4567,21 @@
         <v>700</v>
       </c>
       <c r="M8" t="n">
+        <v>0.1033962928644259</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.009002141732032702</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.807004758154598e-06</v>
+      </c>
+      <c r="P8" t="n">
         <v>34.25747381981383</v>
       </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3990,16 +4590,16 @@
         <v>45591</v>
       </c>
       <c r="B9" t="n">
-        <v>4945.517108443461</v>
+        <v>4938.916536289141</v>
       </c>
       <c r="C9" t="n">
-        <v>4583.328666845399</v>
+        <v>4591.316938915174</v>
       </c>
       <c r="D9" t="n">
-        <v>71.16876975999247</v>
+        <v>71.21276797447767</v>
       </c>
       <c r="E9" t="n">
-        <v>10.04189855144975</v>
+        <v>10.06287683723352</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -4029,12 +4629,21 @@
         <v>655</v>
       </c>
       <c r="M9" t="n">
+        <v>0.1085560487415818</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.007898958582429573</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1.599005207712879e-06</v>
+      </c>
+      <c r="P9" t="n">
         <v>37.71741795240586</v>
       </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4043,16 +4652,16 @@
         <v>43542</v>
       </c>
       <c r="B10" t="n">
-        <v>5140.792412129039</v>
+        <v>5108.401701361344</v>
       </c>
       <c r="C10" t="n">
-        <v>4659.020411590581</v>
+        <v>4625.399182536383</v>
       </c>
       <c r="D10" t="n">
-        <v>73.76992070468908</v>
+        <v>74.1809236590499</v>
       </c>
       <c r="E10" t="n">
-        <v>9.724216846663401</v>
+        <v>9.732278894308605</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -4082,12 +4691,21 @@
         <v>167</v>
       </c>
       <c r="M10" t="n">
+        <v>0.4415531170181541</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.02700386061564189</v>
+      </c>
+      <c r="O10" t="n">
+        <v>5.285117678106876e-06</v>
+      </c>
+      <c r="P10" t="n">
         <v>11.68531416223404</v>
       </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
AFT no funcionando bien xd
</commit_message>
<xml_diff>
--- a/Datos/database.xlsx
+++ b/Datos/database.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,20 +498,45 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>TPH_acum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>dias_230</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ratio_tph_caudal</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>solido_presion</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>E</t>
         </is>
@@ -522,16 +547,16 @@
         <v>43542</v>
       </c>
       <c r="B2" t="n">
-        <v>3547.089913296174</v>
+        <v>3597.082433398252</v>
       </c>
       <c r="C2" t="n">
-        <v>4431.989957678732</v>
+        <v>4411.41003994236</v>
       </c>
       <c r="D2" t="n">
-        <v>70.14103734484949</v>
+        <v>70.73372416587952</v>
       </c>
       <c r="E2" t="n">
-        <v>9.738539620362415</v>
+        <v>9.834484852220104</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -555,18 +580,33 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2365.5419921875</v>
+        <v>7.769185093616296</v>
       </c>
       <c r="L2" t="n">
+        <v>17645.64015976944</v>
+      </c>
+      <c r="M2" t="n">
         <v>196</v>
       </c>
-      <c r="M2" t="n">
-        <v>9.856424967447916</v>
-      </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>806.616845359685</v>
       </c>
       <c r="O2" t="n">
+        <v>3569.200270332795</v>
+      </c>
+      <c r="P2" t="n">
+        <v>1.22638558035795</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>695.6297388504573</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.03237160455673457</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -608,18 +648,33 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>148.064453125</v>
+        <v>5.004378783722188</v>
       </c>
       <c r="L3" t="n">
+        <v>9437.123046875</v>
+      </c>
+      <c r="M3" t="n">
         <v>18</v>
       </c>
-      <c r="M3" t="n">
-        <v>0.6341090069593148</v>
-      </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>992.0970279180862</v>
       </c>
       <c r="O3" t="n">
+        <v>1534.345462901612</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.8398460269563586</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>624.5665219811145</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.02143202905234342</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -628,16 +683,16 @@
         <v>43046</v>
       </c>
       <c r="B4" t="n">
-        <v>3569.976554842808</v>
+        <v>3670.201486548581</v>
       </c>
       <c r="C4" t="n">
-        <v>4801.625823027805</v>
+        <v>4837.450935228825</v>
       </c>
       <c r="D4" t="n">
-        <v>69.65442779912708</v>
+        <v>69.52377413023304</v>
       </c>
       <c r="E4" t="n">
-        <v>9.867431660060207</v>
+        <v>9.905014839610125</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -661,18 +716,33 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>1195.0048828125</v>
+        <v>7.086742017121391</v>
       </c>
       <c r="L4" t="n">
+        <v>9674.90187045765</v>
+      </c>
+      <c r="M4" t="n">
         <v>56</v>
       </c>
-      <c r="M4" t="n">
-        <v>5.085127160904255</v>
-      </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>859.7253873443234</v>
       </c>
       <c r="O4" t="n">
+        <v>2035.672277815865</v>
+      </c>
+      <c r="P4" t="n">
+        <v>1.318034156919699</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>688.6340144656607</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.03015634900902719</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -681,16 +751,16 @@
         <v>43997</v>
       </c>
       <c r="B5" t="n">
-        <v>3665.670568011524</v>
+        <v>3729.695812561793</v>
       </c>
       <c r="C5" t="n">
-        <v>4105.001672883463</v>
+        <v>4095.470162633983</v>
       </c>
       <c r="D5" t="n">
-        <v>69.65747442500769</v>
+        <v>69.79648451757609</v>
       </c>
       <c r="E5" t="n">
-        <v>9.777703092005542</v>
+        <v>9.795065409657823</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -714,18 +784,33 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>3748.732421875</v>
+        <v>8.22943976225196</v>
       </c>
       <c r="L5" t="n">
+        <v>8190.940325267967</v>
+      </c>
+      <c r="M5" t="n">
         <v>251</v>
       </c>
-      <c r="M5" t="n">
-        <v>15.61971842447917</v>
-      </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>756.2374999514155</v>
       </c>
       <c r="O5" t="n">
+        <v>1511.840380489261</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.098070823325467</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>683.6611312138274</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.0342893323427165</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -734,13 +819,13 @@
         <v>45545</v>
       </c>
       <c r="B6" t="n">
-        <v>4974.534009767476</v>
+        <v>4954.049216695412</v>
       </c>
       <c r="C6" t="n">
         <v>4812.063802083333</v>
       </c>
       <c r="D6" t="n">
-        <v>63.13250479345356</v>
+        <v>62.94833103747705</v>
       </c>
       <c r="E6" t="n">
         <v>7.701962391535442</v>
@@ -767,18 +852,33 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>466.740234375</v>
+        <v>6.147913087063458</v>
       </c>
       <c r="L6" t="n">
+        <v>14436.19140625</v>
+      </c>
+      <c r="M6" t="n">
         <v>41</v>
       </c>
-      <c r="M6" t="n">
-        <v>2.007484879032258</v>
-      </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>880.6532797859999</v>
       </c>
       <c r="O6" t="n">
+        <v>2361.581206513397</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.9713395208414614</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>484.8256782605715</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.02644263693360627</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -787,16 +887,16 @@
         <v>43542</v>
       </c>
       <c r="B7" t="n">
-        <v>3498.790380821041</v>
+        <v>3541.977892450911</v>
       </c>
       <c r="C7" t="n">
         <v>4612.53173828125</v>
       </c>
       <c r="D7" t="n">
-        <v>70.71662305833769</v>
+        <v>70.78682316924385</v>
       </c>
       <c r="E7" t="n">
-        <v>9.76184226482906</v>
+        <v>9.782297352122502</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -820,18 +920,33 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>640.8544921875</v>
+        <v>6.464361630318471</v>
       </c>
       <c r="L7" t="n">
+        <v>9225.0634765625</v>
+      </c>
+      <c r="M7" t="n">
         <v>70</v>
       </c>
-      <c r="M7" t="n">
-        <v>2.67022705078125</v>
-      </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>948.3305696460968</v>
       </c>
       <c r="O7" t="n">
+        <v>2187.968176940222</v>
+      </c>
+      <c r="P7" t="n">
+        <v>1.302247463229389</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>692.4577528536578</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.02693484012632696</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -840,16 +955,16 @@
         <v>43375</v>
       </c>
       <c r="B8" t="n">
-        <v>3614.839368995646</v>
+        <v>3677.648353107669</v>
       </c>
       <c r="C8" t="n">
-        <v>4177.049961369733</v>
+        <v>4174.916072061043</v>
       </c>
       <c r="D8" t="n">
-        <v>71.36835185764457</v>
+        <v>71.76215980254851</v>
       </c>
       <c r="E8" t="n">
-        <v>9.709000910803288</v>
+        <v>9.792608333192032</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -873,72 +988,34 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>7173.14453125</v>
+        <v>8.878238804425392</v>
       </c>
       <c r="L8" t="n">
+        <v>20874.58036030521</v>
+      </c>
+      <c r="M8" t="n">
         <v>385</v>
       </c>
-      <c r="M8" t="n">
-        <v>29.88810221354167</v>
-      </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>726.4671488848751</v>
       </c>
       <c r="O8" t="n">
+        <v>3762.03963294156</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1.135213500546087</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>702.7387240902948</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.0369926616851058</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>45522</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5618.364990234375</v>
-      </c>
-      <c r="C9" t="n">
-        <v>4718.5615234375</v>
-      </c>
-      <c r="D9" t="n">
-        <v>59.56926345825195</v>
-      </c>
-      <c r="E9" t="n">
-        <v>10.48471117019653</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>BHC 1011</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> CyC</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>233.5</v>
-      </c>
-      <c r="I9" t="n">
-        <v>51591.744140625</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>1011 CyC_2024-07-31</t>
-        </is>
-      </c>
-      <c r="K9" t="n">
-        <v>36.37890625</v>
-      </c>
-      <c r="L9" t="n">
-        <v>18</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.1557983137044968</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +1029,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1018,20 +1095,45 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>TPH_acum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>dias_230</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ratio_tph_caudal</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>solido_presion</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>E</t>
         </is>
@@ -1042,16 +1144,16 @@
         <v>43164</v>
       </c>
       <c r="B2" t="n">
-        <v>4822.20278020622</v>
+        <v>4717.24350912809</v>
       </c>
       <c r="C2" t="n">
-        <v>4569.182270489694</v>
+        <v>4535.301102700781</v>
       </c>
       <c r="D2" t="n">
-        <v>71.69795450573936</v>
+        <v>71.85949463813277</v>
       </c>
       <c r="E2" t="n">
-        <v>10.05085237051475</v>
+        <v>10.08010168156117</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1075,18 +1177,33 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>2396.73828125</v>
+        <v>7.782281189201685</v>
       </c>
       <c r="L2" t="n">
+        <v>13605.90330810234</v>
+      </c>
+      <c r="M2" t="n">
         <v>174</v>
       </c>
-      <c r="M2" t="n">
-        <v>9.986409505208334</v>
-      </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>818.2326788453109</v>
       </c>
       <c r="O2" t="n">
+        <v>2175.878354242684</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.9614303531947108</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>724.3510127379778</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.03242617162167369</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1128,18 +1245,33 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>1000.4765625</v>
+        <v>6.909230752435628</v>
       </c>
       <c r="L3" t="n">
+        <v>9225.0634765625</v>
+      </c>
+      <c r="M3" t="n">
         <v>70</v>
       </c>
-      <c r="M3" t="n">
-        <v>4.257347074468085</v>
-      </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>832.3067269286357</v>
       </c>
       <c r="O3" t="n">
+        <v>1423.69412345001</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.9249822088299008</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>637.5535281647608</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.02940098192525799</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1148,16 +1280,16 @@
         <v>43828</v>
       </c>
       <c r="B4" t="n">
-        <v>5186.355056709255</v>
+        <v>5036.341524207454</v>
       </c>
       <c r="C4" t="n">
-        <v>4829.496429352894</v>
+        <v>4850.526971127314</v>
       </c>
       <c r="D4" t="n">
-        <v>68.79243615296072</v>
+        <v>68.87048761446377</v>
       </c>
       <c r="E4" t="n">
-        <v>9.856226228569037</v>
+        <v>9.922297960726304</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -1181,18 +1313,33 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>976.091796875</v>
+        <v>6.884580605535873</v>
       </c>
       <c r="L4" t="n">
+        <v>9701.053942254628</v>
+      </c>
+      <c r="M4" t="n">
         <v>82</v>
       </c>
-      <c r="M4" t="n">
-        <v>4.067049153645834</v>
-      </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>873.4832080492506</v>
       </c>
       <c r="O4" t="n">
+        <v>1551.265489061018</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.9631052497496319</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>683.3534988112201</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.02868575252306614</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1207,7 +1354,7 @@
         <v>4754.181396484375</v>
       </c>
       <c r="D5" t="n">
-        <v>69.671844935314</v>
+        <v>69.99035214590563</v>
       </c>
       <c r="E5" t="n">
         <v>9.813123226165771</v>
@@ -1234,18 +1381,33 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>1131.416015625</v>
+        <v>7.032108696218799</v>
       </c>
       <c r="L5" t="n">
+        <v>9508.36279296875</v>
+      </c>
+      <c r="M5" t="n">
         <v>71</v>
       </c>
-      <c r="M5" t="n">
-        <v>4.7142333984375</v>
-      </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>871.3820341955076</v>
       </c>
       <c r="O5" t="n">
+        <v>1759.415258013825</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.109254312569852</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>686.8239502505079</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.02930045290091166</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1254,16 +1416,16 @@
         <v>43375</v>
       </c>
       <c r="B6" t="n">
-        <v>5115.630591800684</v>
+        <v>5151.844864473986</v>
       </c>
       <c r="C6" t="n">
-        <v>4477.78958947218</v>
+        <v>4486.707993541592</v>
       </c>
       <c r="D6" t="n">
         <v>78.40909576416016</v>
       </c>
       <c r="E6" t="n">
-        <v>9.817621248318309</v>
+        <v>9.803691072292432</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -1287,18 +1449,33 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>1230.2158203125</v>
+        <v>7.115757431948694</v>
       </c>
       <c r="L6" t="n">
+        <v>13460.12398062478</v>
+      </c>
+      <c r="M6" t="n">
         <v>80</v>
       </c>
-      <c r="M6" t="n">
-        <v>5.125899251302084</v>
-      </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>966.1340475196184</v>
       </c>
       <c r="O6" t="n">
+        <v>2313.072168878248</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.8708934571714361</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>768.6985521296193</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.02964898929978622</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1340,18 +1517,33 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>1346.7919921875</v>
+        <v>7.20622297109923</v>
       </c>
       <c r="L7" t="n">
+        <v>9225.0634765625</v>
+      </c>
+      <c r="M7" t="n">
         <v>70</v>
       </c>
-      <c r="M7" t="n">
-        <v>5.61163330078125</v>
-      </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>802.184632719189</v>
       </c>
       <c r="O7" t="n">
+        <v>1375.824107501255</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.9249822088299008</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>637.5535281647608</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.03002592904624679</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1360,16 +1552,16 @@
         <v>44135</v>
       </c>
       <c r="B8" t="n">
-        <v>4840.398021170243</v>
+        <v>4893.16503414167</v>
       </c>
       <c r="C8" t="n">
         <v>4539.75390625</v>
       </c>
       <c r="D8" t="n">
-        <v>68.3883929705524</v>
+        <v>68.4164920735699</v>
       </c>
       <c r="E8" t="n">
-        <v>9.944523359764183</v>
+        <v>9.917585619377222</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1393,18 +1585,33 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>4869.677368164059</v>
+        <v>8.490988296376608</v>
       </c>
       <c r="L8" t="n">
+        <v>18159.015625</v>
+      </c>
+      <c r="M8" t="n">
         <v>307</v>
       </c>
-      <c r="M8" t="n">
-        <v>20.29032236735025</v>
-      </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>720.8574063850588</v>
       </c>
       <c r="O8" t="n">
+        <v>2495.083222373334</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.9277745314732864</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>678.5264179170725</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.0353791179015692</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1446,18 +1653,33 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>873.734375</v>
+        <v>6.773920268841909</v>
       </c>
       <c r="L9" t="n">
+        <v>8795.608642578125</v>
+      </c>
+      <c r="M9" t="n">
         <v>51</v>
       </c>
-      <c r="M9" t="n">
-        <v>3.640559895833333</v>
-      </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1008.617184799618</v>
       </c>
       <c r="O9" t="n">
+        <v>1523.806850224697</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.8249316567906904</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>769.8354823865629</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.02822466778684129</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1499,18 +1721,33 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>908.111328125</v>
+        <v>6.81246755986307</v>
       </c>
       <c r="L10" t="n">
+        <v>9225.0634765625</v>
+      </c>
+      <c r="M10" t="n">
         <v>70</v>
       </c>
-      <c r="M10" t="n">
-        <v>3.86430352393617</v>
-      </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>842.6154617144276</v>
       </c>
       <c r="O10" t="n">
+        <v>1440.019872384623</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.9249822088299008</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>637.5535281647608</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.02898922365899179</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1519,16 +1756,16 @@
         <v>43542</v>
       </c>
       <c r="B11" t="n">
-        <v>5203.495308921175</v>
+        <v>5221.602445257827</v>
       </c>
       <c r="C11" t="n">
-        <v>4239.589008603278</v>
+        <v>4244.048210637983</v>
       </c>
       <c r="D11" t="n">
         <v>74.21575037638347</v>
       </c>
       <c r="E11" t="n">
-        <v>9.687354414340632</v>
+        <v>9.680389326327694</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1552,18 +1789,33 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>3248.748046875</v>
+        <v>8.086332748280178</v>
       </c>
       <c r="L11" t="n">
+        <v>25464.2892638279</v>
+      </c>
+      <c r="M11" t="n">
         <v>292</v>
       </c>
-      <c r="M11" t="n">
-        <v>13.5364501953125</v>
-      </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>816.7844215305752</v>
       </c>
       <c r="O11" t="n">
+        <v>3700.130931266399</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.8127865434038343</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>718.437357788943</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.03369305311783408</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1572,16 +1824,16 @@
         <v>44060</v>
       </c>
       <c r="B12" t="n">
-        <v>5003.190688383241</v>
+        <v>5073.546705678476</v>
       </c>
       <c r="C12" t="n">
         <v>4490.618815104167</v>
       </c>
       <c r="D12" t="n">
-        <v>68.82377058345789</v>
+        <v>68.86123605414788</v>
       </c>
       <c r="E12" t="n">
-        <v>9.918243441884471</v>
+        <v>9.882326454701856</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1605,18 +1857,33 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>3101.87109375</v>
+        <v>8.040083121126557</v>
       </c>
       <c r="L12" t="n">
+        <v>13471.8564453125</v>
+      </c>
+      <c r="M12" t="n">
         <v>232</v>
       </c>
-      <c r="M12" t="n">
-        <v>12.924462890625</v>
-      </c>
       <c r="N12" t="n">
-        <v>0</v>
+        <v>761.7323328943743</v>
       </c>
       <c r="O12" t="n">
+        <v>1884.12320150917</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.8851044578395382</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>680.5092147613748</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.03350034633802732</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1631,7 +1898,7 @@
         <v>4405.142415364583</v>
       </c>
       <c r="D13" t="n">
-        <v>69.70299498486054</v>
+        <v>69.89608167019996</v>
       </c>
       <c r="E13" t="n">
         <v>9.929780324300131</v>
@@ -1658,18 +1925,33 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>1677.6533203125</v>
+        <v>7.425747155896115</v>
       </c>
       <c r="L13" t="n">
+        <v>13215.42724609375</v>
+      </c>
+      <c r="M13" t="n">
         <v>110</v>
       </c>
-      <c r="M13" t="n">
-        <v>7.18481079362955</v>
-      </c>
       <c r="N13" t="n">
-        <v>0</v>
+        <v>829.5535146849088</v>
       </c>
       <c r="O13" t="n">
+        <v>2268.257100966686</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.9945534375664119</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>694.0527365144266</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.03180191501454439</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
+      <c r="T13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1684,7 +1966,7 @@
         <v>3991.271240234375</v>
       </c>
       <c r="D14" t="n">
-        <v>70.26625117305336</v>
+        <v>70.44854089310788</v>
       </c>
       <c r="E14" t="n">
         <v>9.812788645426433</v>
@@ -1711,36 +1993,51 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>1031.33203125</v>
+        <v>6.939575630003039</v>
       </c>
       <c r="L14" t="n">
+        <v>11973.81372070312</v>
+      </c>
+      <c r="M14" t="n">
         <v>56</v>
       </c>
-      <c r="M14" t="n">
-        <v>4.370050979872881</v>
-      </c>
       <c r="N14" t="n">
-        <v>0</v>
+        <v>887.3086443926338</v>
       </c>
       <c r="O14" t="n">
+        <v>2322.59629801676</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.9631277307088664</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>691.2966421627488</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.02940498148306372</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>43164</v>
+        <v>43746</v>
       </c>
       <c r="B15" t="n">
-        <v>4819.647636289437</v>
+        <v>4867.842989051204</v>
       </c>
       <c r="C15" t="n">
-        <v>4401.077116672041</v>
+        <v>4716.259148861689</v>
       </c>
       <c r="D15" t="n">
-        <v>74.11153747149966</v>
+        <v>68.22744791109463</v>
       </c>
       <c r="E15" t="n">
-        <v>9.764426577470124</v>
+        <v>9.739918238131089</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1753,47 +2050,62 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="I15" t="n">
-        <v>12689.7333984375</v>
+        <v>20669.765625</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1012 CyF_2017-11-07</t>
+          <t>1012 CyF_2019-03-18</t>
         </is>
       </c>
       <c r="K15" t="n">
-        <v>0.669921875</v>
+        <v>7.729741340982378</v>
       </c>
       <c r="L15" t="n">
-        <v>118</v>
+        <v>9432.518297723378</v>
       </c>
       <c r="M15" t="n">
-        <v>0.002850731382978723</v>
+        <v>204</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>781.5517693610935</v>
       </c>
       <c r="O15" t="n">
+        <v>1404.210338471735</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0.9688601603997786</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>664.5297642504095</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.03346208372719644</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
+      <c r="T15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>43746</v>
+        <v>45199</v>
       </c>
       <c r="B16" t="n">
-        <v>5017.856521553005</v>
+        <v>4268.611653645833</v>
       </c>
       <c r="C16" t="n">
-        <v>4695.228607087269</v>
+        <v>4655.380696614583</v>
       </c>
       <c r="D16" t="n">
-        <v>68.14939644959158</v>
+        <v>69.91856781145316</v>
       </c>
       <c r="E16" t="n">
-        <v>9.673846505973822</v>
+        <v>9.917221069335938</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1806,47 +2118,62 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="I16" t="n">
-        <v>20669.765625</v>
+        <v>29355.20458984375</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>1012 CyF_2019-03-18</t>
+          <t>1012 CyF_2023-07-13</t>
         </is>
       </c>
       <c r="K16" t="n">
-        <v>2274.013671875</v>
+        <v>5.620240746184468</v>
       </c>
       <c r="L16" t="n">
-        <v>204</v>
+        <v>13966.14208984375</v>
       </c>
       <c r="M16" t="n">
-        <v>9.844215029761905</v>
+        <v>79</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>1056.133311341438</v>
       </c>
       <c r="O16" t="n">
+        <v>3086.932557411591</v>
+      </c>
+      <c r="P16" t="n">
+        <v>1.09060768780227</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>693.3978938375368</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.02401812284694217</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0</v>
+      </c>
+      <c r="T16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45199</v>
+        <v>45471</v>
       </c>
       <c r="B17" t="n">
-        <v>4268.611653645833</v>
+        <v>4381.087076822917</v>
       </c>
       <c r="C17" t="n">
-        <v>4655.380696614583</v>
+        <v>4027.862711588542</v>
       </c>
       <c r="D17" t="n">
-        <v>69.62294164051559</v>
+        <v>70.22492466222972</v>
       </c>
       <c r="E17" t="n">
-        <v>9.917221069335938</v>
+        <v>9.550990104675293</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1859,47 +2186,62 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>234</v>
+        <v>233.5</v>
       </c>
       <c r="I17" t="n">
-        <v>29355.20458984375</v>
+        <v>30841.90478515625</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>1012 CyF_2023-07-13</t>
+          <t>1012 CyF_2024-05-17</t>
         </is>
       </c>
       <c r="K17" t="n">
-        <v>274.9558105468714</v>
+        <v>5.965714704704492</v>
       </c>
       <c r="L17" t="n">
-        <v>79</v>
+        <v>12083.58813476562</v>
       </c>
       <c r="M17" t="n">
-        <v>1.175024831396886</v>
+        <v>42</v>
       </c>
       <c r="N17" t="n">
-        <v>0</v>
+        <v>1008.151031721143</v>
       </c>
       <c r="O17" t="n">
+        <v>2502.081500605598</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.9193751760158397</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>670.717560550524</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.02554909937774943</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0</v>
+      </c>
+      <c r="T17" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45471</v>
+        <v>43046</v>
       </c>
       <c r="B18" t="n">
-        <v>4381.087076822917</v>
+        <v>4723.040085233353</v>
       </c>
       <c r="C18" t="n">
-        <v>4027.862711588542</v>
+        <v>4792.585565183983</v>
       </c>
       <c r="D18" t="n">
-        <v>69.69423547190523</v>
+        <v>68.58469407511907</v>
       </c>
       <c r="E18" t="n">
-        <v>9.550990104675293</v>
+        <v>10.20331325385559</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1908,51 +2250,66 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CyF</t>
+          <t xml:space="preserve"> CyG</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>233.5</v>
+        <v>240</v>
       </c>
       <c r="I18" t="n">
-        <v>30841.90478515625</v>
+        <v>11754.7451171875</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1012 CyF_2024-05-17</t>
+          <t>1012 CyG_2017-09-12</t>
         </is>
       </c>
       <c r="K18" t="n">
-        <v>388.83154296875</v>
+        <v>6.909551516343956</v>
       </c>
       <c r="L18" t="n">
-        <v>42</v>
+        <v>9585.171130367966</v>
       </c>
       <c r="M18" t="n">
-        <v>1.66523144740364</v>
+        <v>56</v>
       </c>
       <c r="N18" t="n">
-        <v>0</v>
+        <v>867.1123000260967</v>
       </c>
       <c r="O18" t="n">
-        <v>0</v>
+        <v>1615.302944087797</v>
+      </c>
+      <c r="P18" t="n">
+        <v>1.014724725716561</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>699.7911180682936</v>
+      </c>
+      <c r="R18" t="n">
+        <v>0.02878979798476648</v>
+      </c>
+      <c r="S18" t="n">
+        <v>0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>43046</v>
+        <v>43472</v>
       </c>
       <c r="B19" t="n">
-        <v>4814.29420610354</v>
+        <v>4751.556115070353</v>
       </c>
       <c r="C19" t="n">
-        <v>4843.407316867354</v>
+        <v>4624.529641679575</v>
       </c>
       <c r="D19" t="n">
-        <v>68.34238387652896</v>
+        <v>72.18566513061523</v>
       </c>
       <c r="E19" t="n">
-        <v>10.20294585485883</v>
+        <v>9.768743757944264</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1968,44 +2325,59 @@
         <v>240</v>
       </c>
       <c r="I19" t="n">
-        <v>11754.7451171875</v>
+        <v>19089.39453125</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>1012 CyG_2017-09-12</t>
+          <t>1012 CyG_2018-10-02</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>1000.7978515625</v>
+        <v>7.638406142049746</v>
       </c>
       <c r="L19" t="n">
-        <v>56</v>
+        <v>9249.059283359151</v>
       </c>
       <c r="M19" t="n">
-        <v>4.169991048177083</v>
+        <v>97</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>835.6363887457462</v>
       </c>
       <c r="O19" t="n">
+        <v>1498.100538480743</v>
+      </c>
+      <c r="P19" t="n">
+        <v>0.9732663405319879</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>705.1632656577525</v>
+      </c>
+      <c r="R19" t="n">
+        <v>0.03182669225854061</v>
+      </c>
+      <c r="S19" t="n">
+        <v>0</v>
+      </c>
+      <c r="T19" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>43472</v>
+        <v>45026</v>
       </c>
       <c r="B20" t="n">
-        <v>4697.234706060401</v>
+        <v>4526.908081054688</v>
       </c>
       <c r="C20" t="n">
-        <v>4611.152035575457</v>
+        <v>4378.823974609375</v>
       </c>
       <c r="D20" t="n">
-        <v>72.18566513061523</v>
+        <v>69.95662293402584</v>
       </c>
       <c r="E20" t="n">
-        <v>9.78963902198308</v>
+        <v>9.831962108612061</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2018,47 +2390,62 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>240</v>
+        <v>232.75</v>
       </c>
       <c r="I20" t="n">
-        <v>19089.39453125</v>
+        <v>42210.4326171875</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1012 CyG_2018-10-02</t>
+          <t>1012 CyG_2023-03-25</t>
         </is>
       </c>
       <c r="K20" t="n">
-        <v>2075.431640625</v>
+        <v>5.794628990261461</v>
       </c>
       <c r="L20" t="n">
-        <v>97</v>
+        <v>8757.64794921875</v>
       </c>
       <c r="M20" t="n">
-        <v>8.647631835937499</v>
+        <v>16</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>1029.587090543024</v>
       </c>
       <c r="O20" t="n">
-        <v>1</v>
+        <v>1794.332221760007</v>
+      </c>
+      <c r="P20" t="n">
+        <v>0.9672880223174994</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>687.8108659338036</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.02489636515686986</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45026</v>
+        <v>43164</v>
       </c>
       <c r="B21" t="n">
-        <v>4526.908081054688</v>
+        <v>4750.106803342549</v>
       </c>
       <c r="C21" t="n">
-        <v>4378.823974609375</v>
+        <v>4350.25536498867</v>
       </c>
       <c r="D21" t="n">
-        <v>69.79192495183143</v>
+        <v>74.35384767008978</v>
       </c>
       <c r="E21" t="n">
-        <v>9.831962108612061</v>
+        <v>9.808300544039753</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2067,51 +2454,66 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CyG</t>
+          <t xml:space="preserve"> CyH</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>232.75</v>
+        <v>235</v>
       </c>
       <c r="I21" t="n">
-        <v>42210.4326171875</v>
+        <v>14855.28515625</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1012 CyG_2023-03-25</t>
+          <t>1012 CyH_2017-11-07</t>
         </is>
       </c>
       <c r="K21" t="n">
-        <v>327.5302734375</v>
+        <v>7.522314138071954</v>
       </c>
       <c r="L21" t="n">
-        <v>16</v>
+        <v>8700.510729977341</v>
       </c>
       <c r="M21" t="n">
-        <v>1.407219219924812</v>
+        <v>118</v>
       </c>
       <c r="N21" t="n">
-        <v>0</v>
+        <v>872.4607713992485</v>
       </c>
       <c r="O21" t="n">
+        <v>1466.807446569399</v>
+      </c>
+      <c r="P21" t="n">
+        <v>0.9158226406128936</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>729.2848845539904</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.03200984739605087</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T21" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>43164</v>
+        <v>43375</v>
       </c>
       <c r="B22" t="n">
-        <v>4819.647636289437</v>
+        <v>5339.095318277365</v>
       </c>
       <c r="C22" t="n">
-        <v>4401.077116672041</v>
+        <v>4059.80644681635</v>
       </c>
       <c r="D22" t="n">
-        <v>74.11153747149966</v>
+        <v>78.40909576416016</v>
       </c>
       <c r="E22" t="n">
-        <v>9.764426577470124</v>
+        <v>9.678090932240565</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2124,47 +2526,62 @@
         </is>
       </c>
       <c r="H22" t="n">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="I22" t="n">
-        <v>14855.28515625</v>
+        <v>18128.314453125</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1012 CyH_2017-11-07</t>
+          <t>1012 CyH_2018-05-30</t>
         </is>
       </c>
       <c r="K22" t="n">
-        <v>1847.8408203125</v>
+        <v>7.357483952605354</v>
       </c>
       <c r="L22" t="n">
-        <v>118</v>
+        <v>16239.2257872654</v>
       </c>
       <c r="M22" t="n">
-        <v>7.863152426861702</v>
+        <v>125</v>
       </c>
       <c r="N22" t="n">
-        <v>0</v>
+        <v>938.1902042386452</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>2628.374468279393</v>
+      </c>
+      <c r="P22" t="n">
+        <v>0.7603922007750008</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>758.8503587203005</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0.03065618313585564</v>
+      </c>
+      <c r="S22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>43375</v>
+        <v>43828</v>
       </c>
       <c r="B23" t="n">
-        <v>5311.934613772388</v>
+        <v>5011.479111713103</v>
       </c>
       <c r="C23" t="n">
-        <v>4053.117643764291</v>
+        <v>4731.529354704282</v>
       </c>
       <c r="D23" t="n">
-        <v>78.40909576416016</v>
+        <v>67.34977360764692</v>
       </c>
       <c r="E23" t="n">
-        <v>9.688538564259972</v>
+        <v>9.803642037614129</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2180,44 +2597,59 @@
         <v>240</v>
       </c>
       <c r="I23" t="n">
-        <v>18128.314453125</v>
+        <v>24510.701171875</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>1012 CyH_2018-05-30</t>
+          <t>1012 CyH_2019-01-07</t>
         </is>
       </c>
       <c r="K23" t="n">
-        <v>1566.88671875</v>
+        <v>8.437596868473211</v>
       </c>
       <c r="L23" t="n">
-        <v>125</v>
+        <v>18926.11741881713</v>
       </c>
       <c r="M23" t="n">
-        <v>6.528694661458333</v>
+        <v>356</v>
       </c>
       <c r="N23" t="n">
-        <v>0</v>
+        <v>713.6326603717562</v>
       </c>
       <c r="O23" t="n">
+        <v>2519.181700459539</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0.9441382952597988</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>660.273071763722</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.03515665361863838</v>
+      </c>
+      <c r="S23" t="n">
+        <v>0</v>
+      </c>
+      <c r="T23" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>43828</v>
+        <v>45429</v>
       </c>
       <c r="B24" t="n">
-        <v>5086.485877964003</v>
+        <v>4452.680324391278</v>
       </c>
       <c r="C24" t="n">
-        <v>4721.014083817072</v>
+        <v>4580.375390625</v>
       </c>
       <c r="D24" t="n">
-        <v>67.31074787689539</v>
+        <v>69.86925438874717</v>
       </c>
       <c r="E24" t="n">
-        <v>9.770606171535494</v>
+        <v>9.697959103700729</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2230,47 +2662,62 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>240</v>
+        <v>237.5</v>
       </c>
       <c r="I24" t="n">
-        <v>24510.701171875</v>
+        <v>47310.94921875</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>1012 CyH_2019-01-07</t>
+          <t>1012 CyH_2023-09-30</t>
         </is>
       </c>
       <c r="K24" t="n">
-        <v>4616.4453125</v>
+        <v>7.991585013985184</v>
       </c>
       <c r="L24" t="n">
-        <v>356</v>
+        <v>22901.876953125</v>
       </c>
       <c r="M24" t="n">
-        <v>19.23518880208333</v>
+        <v>230</v>
       </c>
       <c r="N24" t="n">
-        <v>0</v>
+        <v>777.0515907937819</v>
       </c>
       <c r="O24" t="n">
-        <v>1</v>
+        <v>3683.089476543796</v>
+      </c>
+      <c r="P24" t="n">
+        <v>1.02867824470745</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>677.5891716681327</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.0336487790062534</v>
+      </c>
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45429</v>
+        <v>45504</v>
       </c>
       <c r="B25" t="n">
-        <v>4470.508316552612</v>
+        <v>4144.072591145833</v>
       </c>
       <c r="C25" t="n">
-        <v>4580.375390625</v>
+        <v>3991.271240234375</v>
       </c>
       <c r="D25" t="n">
-        <v>69.60416014378731</v>
+        <v>70.44854089310788</v>
       </c>
       <c r="E25" t="n">
-        <v>9.743335280526924</v>
+        <v>9.812788645426433</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2283,47 +2730,62 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>237.5</v>
+        <v>235</v>
       </c>
       <c r="I25" t="n">
-        <v>47310.94921875</v>
+        <v>48206.03515625</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>1012 CyH_2023-09-30</t>
+          <t>1012 CyH_2024-06-05</t>
         </is>
       </c>
       <c r="K25" t="n">
-        <v>2954.978515625</v>
+        <v>6.547342890741401</v>
       </c>
       <c r="L25" t="n">
-        <v>230</v>
+        <v>11973.81372070312</v>
       </c>
       <c r="M25" t="n">
-        <v>12.44201480263158</v>
+        <v>56</v>
       </c>
       <c r="N25" t="n">
-        <v>0</v>
+        <v>933.4217606507536</v>
       </c>
       <c r="O25" t="n">
+        <v>2431.816056037621</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0.9631277307088664</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>691.2966421627488</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.02786103357762298</v>
+      </c>
+      <c r="S25" t="n">
+        <v>0</v>
+      </c>
+      <c r="T25" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45504</v>
+        <v>43250</v>
       </c>
       <c r="B26" t="n">
-        <v>4144.072591145833</v>
+        <v>5013.144301767943</v>
       </c>
       <c r="C26" t="n">
-        <v>3991.271240234375</v>
+        <v>4096.251278685741</v>
       </c>
       <c r="D26" t="n">
-        <v>70.26625117305336</v>
+        <v>73.49689491963962</v>
       </c>
       <c r="E26" t="n">
-        <v>9.812788645426433</v>
+        <v>9.885398889192116</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2332,51 +2794,66 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CyH</t>
+          <t xml:space="preserve"> CyI</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="I26" t="n">
-        <v>48206.03515625</v>
+        <v>19021.04296875</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1012 CyH_2024-06-05</t>
+          <t>1012 CyI_2017-09-12</t>
         </is>
       </c>
       <c r="K26" t="n">
-        <v>696.388671875</v>
+        <v>8.520328700254122</v>
       </c>
       <c r="L26" t="n">
-        <v>56</v>
+        <v>16385.00511474297</v>
       </c>
       <c r="M26" t="n">
-        <v>2.963356050531915</v>
+        <v>260</v>
       </c>
       <c r="N26" t="n">
-        <v>0</v>
+        <v>771.9995520498971</v>
       </c>
       <c r="O26" t="n">
-        <v>0</v>
+        <v>2346.386631687724</v>
+      </c>
+      <c r="P26" t="n">
+        <v>0.8171022065074268</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>726.5461233976752</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.03550136958439218</v>
+      </c>
+      <c r="S26" t="n">
+        <v>0</v>
+      </c>
+      <c r="T26" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>43250</v>
+        <v>43472</v>
       </c>
       <c r="B27" t="n">
-        <v>5091.86375507654</v>
+        <v>5041.33482023049</v>
       </c>
       <c r="C27" t="n">
-        <v>4121.662154527427</v>
+        <v>4511.166981484319</v>
       </c>
       <c r="D27" t="n">
-        <v>73.37573982034456</v>
+        <v>75.2973804473877</v>
       </c>
       <c r="E27" t="n">
-        <v>9.863461905907302</v>
+        <v>9.793467404713709</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2392,44 +2869,59 @@
         <v>240</v>
       </c>
       <c r="I27" t="n">
-        <v>19021.04296875</v>
+        <v>21926.11328125</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>1012 CyI_2017-09-12</t>
+          <t>1012 CyI_2018-07-14</t>
         </is>
       </c>
       <c r="K27" t="n">
-        <v>5014.7021484375</v>
+        <v>7.71357087530081</v>
       </c>
       <c r="L27" t="n">
-        <v>260</v>
+        <v>18044.66792593728</v>
       </c>
       <c r="M27" t="n">
-        <v>20.89459228515625</v>
+        <v>177</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
+        <v>864.1391861610155</v>
       </c>
       <c r="O27" t="n">
+        <v>2854.302067422435</v>
+      </c>
+      <c r="P27" t="n">
+        <v>0.8948358189646508</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>737.4224410718188</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0.03213987864708671</v>
+      </c>
+      <c r="S27" t="n">
+        <v>0</v>
+      </c>
+      <c r="T27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>43472</v>
+        <v>43746</v>
       </c>
       <c r="B28" t="n">
-        <v>5014.174115725513</v>
+        <v>4867.842989051204</v>
       </c>
       <c r="C28" t="n">
-        <v>4504.47817843226</v>
+        <v>4716.259148861689</v>
       </c>
       <c r="D28" t="n">
-        <v>75.2973804473877</v>
+        <v>68.22744791109463</v>
       </c>
       <c r="E28" t="n">
-        <v>9.803915036733116</v>
+        <v>9.739918238131089</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2442,47 +2934,62 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>240</v>
+        <v>234.5</v>
       </c>
       <c r="I28" t="n">
-        <v>21926.11328125</v>
+        <v>25128.5625</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1012 CyI_2018-07-14</t>
+          <t>1012 CyI_2019-03-18</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>2237.521484375</v>
+        <v>7.684741737172339</v>
       </c>
       <c r="L28" t="n">
-        <v>177</v>
+        <v>9432.518297723378</v>
       </c>
       <c r="M28" t="n">
-        <v>9.323006184895833</v>
+        <v>204</v>
       </c>
       <c r="N28" t="n">
-        <v>0</v>
+        <v>785.6013451622659</v>
       </c>
       <c r="O28" t="n">
-        <v>1</v>
+        <v>1410.968099314403</v>
+      </c>
+      <c r="P28" t="n">
+        <v>0.9688601603997786</v>
+      </c>
+      <c r="Q28" t="n">
+        <v>664.5297642504095</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.0327707536766411</v>
+      </c>
+      <c r="S28" t="n">
+        <v>0</v>
+      </c>
+      <c r="T28" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>43746</v>
+        <v>45199</v>
       </c>
       <c r="B29" t="n">
-        <v>5017.856521553005</v>
+        <v>4285.925537109375</v>
       </c>
       <c r="C29" t="n">
-        <v>4695.228607087269</v>
+        <v>4754.181396484375</v>
       </c>
       <c r="D29" t="n">
-        <v>68.14939644959158</v>
+        <v>69.99035214590563</v>
       </c>
       <c r="E29" t="n">
-        <v>9.673846505973822</v>
+        <v>9.813123226165771</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2491,86 +2998,48 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> CyI</t>
+          <t xml:space="preserve"> CyJ</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>234.5</v>
+        <v>237.5</v>
       </c>
       <c r="I29" t="n">
-        <v>25128.5625</v>
+        <v>39430.66796875</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>1012 CyI_2019-03-18</t>
+          <t>1012 CyJ_2023-07-21</t>
         </is>
       </c>
       <c r="K29" t="n">
-        <v>2173.908203125</v>
+        <v>6.7136999151677</v>
       </c>
       <c r="L29" t="n">
-        <v>204</v>
+        <v>9508.36279296875</v>
       </c>
       <c r="M29" t="n">
-        <v>9.270397454690832</v>
+        <v>71</v>
       </c>
       <c r="N29" t="n">
-        <v>0</v>
+        <v>907.3512440933996</v>
       </c>
       <c r="O29" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>45199</v>
-      </c>
-      <c r="B30" t="n">
-        <v>4285.925537109375</v>
-      </c>
-      <c r="C30" t="n">
-        <v>4754.181396484375</v>
-      </c>
-      <c r="D30" t="n">
-        <v>69.671844935314</v>
-      </c>
-      <c r="E30" t="n">
-        <v>9.813123226165771</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>BHC 1012</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> CyJ</t>
-        </is>
-      </c>
-      <c r="H30" t="n">
-        <v>237.5</v>
-      </c>
-      <c r="I30" t="n">
-        <v>39430.66796875</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>1012 CyJ_2023-07-21</t>
-        </is>
-      </c>
-      <c r="K30" t="n">
-        <v>822.6123046875</v>
-      </c>
-      <c r="L30" t="n">
-        <v>71</v>
-      </c>
-      <c r="M30" t="n">
-        <v>3.463630756578947</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
+        <v>1825.487585781263</v>
+      </c>
+      <c r="P29" t="n">
+        <v>1.109254312569852</v>
+      </c>
+      <c r="Q29" t="n">
+        <v>686.8239502505079</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.02826821016912716</v>
+      </c>
+      <c r="S29" t="n">
+        <v>0</v>
+      </c>
+      <c r="T29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2585,7 +3054,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2651,20 +3120,45 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>TPH_acum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>dias_230</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ratio_tph_caudal</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>solido_presion</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>E</t>
         </is>
@@ -2675,16 +3169,16 @@
         <v>43746</v>
       </c>
       <c r="B2" t="n">
-        <v>5200.202255968126</v>
+        <v>5216.768892921375</v>
       </c>
       <c r="C2" t="n">
-        <v>4682.084354890255</v>
+        <v>4664.385595703701</v>
       </c>
       <c r="D2" t="n">
         <v>76.89302062988281</v>
       </c>
       <c r="E2" t="n">
-        <v>9.921547643013241</v>
+        <v>9.929870329281636</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2708,18 +3202,33 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>3599.795654296882</v>
+        <v>8.188910115106433</v>
       </c>
       <c r="L2" t="n">
+        <v>9328.771191407403</v>
+      </c>
+      <c r="M2" t="n">
         <v>204</v>
       </c>
-      <c r="M2" t="n">
-        <v>15.31827937998673</v>
-      </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>836.8024027514625</v>
       </c>
       <c r="O2" t="n">
+        <v>1387.595732777172</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.894113901248656</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>763.5377240815141</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.0348464260217295</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2761,18 +3270,33 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>815.265625</v>
+        <v>6.704739822827029</v>
       </c>
       <c r="L3" t="n">
+        <v>8094.996826171875</v>
+      </c>
+      <c r="M3" t="n">
         <v>62</v>
       </c>
-      <c r="M3" t="n">
-        <v>3.476612473347548</v>
-      </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>1017.673504455732</v>
       </c>
       <c r="O3" t="n">
+        <v>2280.176707879604</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.294401913991066</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>808.2622773875516</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.02859164103550972</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2781,7 +3305,7 @@
         <v>43542</v>
       </c>
       <c r="B4" t="n">
-        <v>5155.959869539516</v>
+        <v>5127.444686574054</v>
       </c>
       <c r="C4" t="n">
         <v>4612.53173828125</v>
@@ -2790,7 +3314,7 @@
         <v>43.95745515823364</v>
       </c>
       <c r="E4" t="n">
-        <v>9.946448302948721</v>
+        <v>9.919744410516685</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -2814,18 +3338,33 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>922.162109375</v>
+        <v>6.827804852206838</v>
       </c>
       <c r="L4" t="n">
+        <v>9225.0634765625</v>
+      </c>
+      <c r="M4" t="n">
         <v>70</v>
       </c>
-      <c r="M4" t="n">
-        <v>3.842342122395833</v>
-      </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>561.5553273002332</v>
       </c>
       <c r="O4" t="n">
+        <v>958.5562109246963</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8995770820040542</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>436.046720106426</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.02844918688419516</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2867,18 +3406,33 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>880.91796875</v>
+        <v>6.782099045729089</v>
       </c>
       <c r="L5" t="n">
+        <v>8094.996826171875</v>
+      </c>
+      <c r="M5" t="n">
         <v>62</v>
       </c>
-      <c r="M5" t="n">
-        <v>3.764606704059829</v>
-      </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>1007.557155253531</v>
       </c>
       <c r="O5" t="n">
+        <v>2260.398650361797</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1.294401913991066</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>808.2622773875516</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.02898332925525252</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2887,16 +3441,16 @@
         <v>43542</v>
       </c>
       <c r="B6" t="n">
-        <v>4957.465847921143</v>
+        <v>4924.087797109564</v>
       </c>
       <c r="C6" t="n">
-        <v>4674.797581943872</v>
+        <v>4646.751248136859</v>
       </c>
       <c r="D6" t="n">
-        <v>57.48956817615735</v>
+        <v>57.2381602410801</v>
       </c>
       <c r="E6" t="n">
-        <v>9.88228280200237</v>
+        <v>9.893739399520392</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -2920,18 +3474,33 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>5272.728515625</v>
+        <v>8.570492889597588</v>
       </c>
       <c r="L6" t="n">
+        <v>18587.00499254743</v>
+      </c>
+      <c r="M6" t="n">
         <v>496</v>
       </c>
-      <c r="M6" t="n">
-        <v>22.20096217105263</v>
-      </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>598.06909530536</v>
       </c>
       <c r="O6" t="n">
+        <v>2130.210106402852</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.9436775764696402</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>566.2994411332357</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.03608628585093721</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2940,16 +3509,16 @@
         <v>43472</v>
       </c>
       <c r="B7" t="n">
-        <v>4696.70965101965</v>
+        <v>4762.797001919349</v>
       </c>
       <c r="C7" t="n">
-        <v>4660.636014111371</v>
+        <v>4613.976170679691</v>
       </c>
       <c r="D7" t="n">
-        <v>42.52256886112435</v>
+        <v>41.27902963402865</v>
       </c>
       <c r="E7" t="n">
-        <v>9.845561766783904</v>
+        <v>9.849081457082217</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -2973,18 +3542,33 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>1047.388671875</v>
+        <v>6.9550096662354</v>
       </c>
       <c r="L7" t="n">
+        <v>9227.952341359382</v>
+      </c>
+      <c r="M7" t="n">
         <v>97</v>
       </c>
-      <c r="M7" t="n">
-        <v>4.364119466145834</v>
-      </c>
       <c r="N7" t="n">
-        <v>0</v>
+        <v>518.9060901991763</v>
       </c>
       <c r="O7" t="n">
+        <v>954.1045344221973</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.9687534780786963</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>406.5605253348589</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.0289792069426475</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2993,16 +3577,16 @@
         <v>43746</v>
       </c>
       <c r="B8" t="n">
-        <v>5200.202255968126</v>
+        <v>5216.768892921375</v>
       </c>
       <c r="C8" t="n">
-        <v>4682.084354890255</v>
+        <v>4664.385595703701</v>
       </c>
       <c r="D8" t="n">
         <v>76.89302062988281</v>
       </c>
       <c r="E8" t="n">
-        <v>9.921547643013241</v>
+        <v>9.929870329281636</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -3026,18 +3610,33 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>3529.735595703121</v>
+        <v>8.169261512270278</v>
       </c>
       <c r="L8" t="n">
+        <v>9328.771191407403</v>
+      </c>
+      <c r="M8" t="n">
         <v>204</v>
       </c>
-      <c r="M8" t="n">
-        <v>14.9248862397595</v>
-      </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>838.5955676690517</v>
       </c>
       <c r="O8" t="n">
+        <v>1390.358198978553</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.894113901248656</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>763.5377240815141</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.03454233197577285</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3046,16 +3645,16 @@
         <v>45549</v>
       </c>
       <c r="B9" t="n">
-        <v>3713.138010286288</v>
+        <v>3664.389977163336</v>
       </c>
       <c r="C9" t="n">
         <v>4623.30078125</v>
       </c>
       <c r="D9" t="n">
-        <v>75.47514600200508</v>
+        <v>74.81669784535114</v>
       </c>
       <c r="E9" t="n">
-        <v>10.27340876035354</v>
+        <v>10.22756291988123</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -3079,18 +3678,33 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>467.650390625</v>
+        <v>6.149857054703297</v>
       </c>
       <c r="L9" t="n">
+        <v>13869.90234375</v>
+      </c>
+      <c r="M9" t="n">
         <v>45</v>
       </c>
-      <c r="M9" t="n">
-        <v>2.007083221566524</v>
-      </c>
       <c r="N9" t="n">
-        <v>0</v>
+        <v>1046.408302612644</v>
       </c>
       <c r="O9" t="n">
+        <v>3483.216539297587</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1.26168360830747</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>765.1924846710715</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.02639423628628024</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3099,16 +3713,16 @@
         <v>43542</v>
       </c>
       <c r="B10" t="n">
-        <v>4988.518022554767</v>
+        <v>5032.5762564879</v>
       </c>
       <c r="C10" t="n">
-        <v>4653.930519824247</v>
+        <v>4622.823957536461</v>
       </c>
       <c r="D10" t="n">
-        <v>53.47402773928471</v>
+        <v>52.6450015878876</v>
       </c>
       <c r="E10" t="n">
-        <v>9.91159297635854</v>
+        <v>9.913939436557415</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -3132,18 +3746,33 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>2406.37109375</v>
+        <v>7.786290598625063</v>
       </c>
       <c r="L10" t="n">
+        <v>13868.47187260938</v>
+      </c>
+      <c r="M10" t="n">
         <v>167</v>
       </c>
-      <c r="M10" t="n">
-        <v>10.02654622395833</v>
-      </c>
       <c r="N10" t="n">
-        <v>0</v>
+        <v>599.1720965401013</v>
       </c>
       <c r="O10" t="n">
+        <v>1559.742213390365</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.9185800100676081</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>521.9193573797866</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.03244287749427109</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3152,16 +3781,16 @@
         <v>43472</v>
       </c>
       <c r="B11" t="n">
-        <v>4696.70965101965</v>
+        <v>4762.797001919349</v>
       </c>
       <c r="C11" t="n">
-        <v>4660.636014111371</v>
+        <v>4613.976170679691</v>
       </c>
       <c r="D11" t="n">
-        <v>42.52256886112435</v>
+        <v>41.27902963402865</v>
       </c>
       <c r="E11" t="n">
-        <v>9.845561766783904</v>
+        <v>9.849081457082217</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -3185,18 +3814,33 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>1815.7578125</v>
+        <v>7.504808769748955</v>
       </c>
       <c r="L11" t="n">
+        <v>9227.952341359382</v>
+      </c>
+      <c r="M11" t="n">
         <v>97</v>
       </c>
-      <c r="M11" t="n">
-        <v>7.726628989361702</v>
-      </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>485.3610557459616</v>
       </c>
       <c r="O11" t="n">
+        <v>895.3204274889533</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.9687534780786963</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>406.5605253348589</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.03193535646701683</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3211,7 +3855,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3277,20 +3921,45 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>TPH_acum</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>dias_230</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>solido_uso</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>carga_solidos_efectiva</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>ratio_tph_caudal</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>solido_presion</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>score</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>score_out</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>E</t>
         </is>
@@ -3301,16 +3970,16 @@
         <v>43472</v>
       </c>
       <c r="B2" t="n">
-        <v>5080.088238082546</v>
+        <v>5108.484713314764</v>
       </c>
       <c r="C2" t="n">
-        <v>4760.033473048973</v>
+        <v>4742.640976694644</v>
       </c>
       <c r="D2" t="n">
-        <v>70.90056903019266</v>
+        <v>70.8288589607173</v>
       </c>
       <c r="E2" t="n">
-        <v>9.934229467524872</v>
+        <v>9.948809181108142</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3334,18 +4003,33 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>5492.01171875</v>
+        <v>8.611231966737396</v>
       </c>
       <c r="L2" t="n">
+        <v>18970.56390677858</v>
+      </c>
+      <c r="M2" t="n">
         <v>482</v>
       </c>
-      <c r="M2" t="n">
-        <v>23.37026263297872</v>
-      </c>
       <c r="N2" t="n">
-        <v>0</v>
+        <v>736.9383988009258</v>
       </c>
       <c r="O2" t="n">
+        <v>2555.932154746152</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.9283850757250121</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>704.662802315798</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.03664354028398892</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3354,16 +4038,16 @@
         <v>43542</v>
       </c>
       <c r="B3" t="n">
-        <v>5047.505108199734</v>
+        <v>5075.901583431952</v>
       </c>
       <c r="C3" t="n">
-        <v>4693.815211330224</v>
+        <v>4676.422714975894</v>
       </c>
       <c r="D3" t="n">
-        <v>73.17196566715555</v>
+        <v>73.10025559768019</v>
       </c>
       <c r="E3" t="n">
-        <v>9.745126579417573</v>
+        <v>9.759706293000843</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -3387,18 +4071,33 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>6335.24609375</v>
+        <v>8.754041773293965</v>
       </c>
       <c r="L3" t="n">
+        <v>18705.69085990358</v>
+      </c>
+      <c r="M3" t="n">
         <v>496</v>
       </c>
-      <c r="M3" t="n">
-        <v>26.39685872395833</v>
-      </c>
       <c r="N3" t="n">
-        <v>0</v>
+        <v>749.4355396121504</v>
       </c>
       <c r="O3" t="n">
+        <v>2575.537399864613</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.9212989316079395</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>713.4370245766494</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.03647517405539152</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3407,16 +4106,16 @@
         <v>43472</v>
       </c>
       <c r="B4" t="n">
-        <v>5080.088238082546</v>
+        <v>5108.484713314764</v>
       </c>
       <c r="C4" t="n">
-        <v>4760.033473048973</v>
+        <v>4742.640976694644</v>
       </c>
       <c r="D4" t="n">
-        <v>70.90056903019266</v>
+        <v>70.8288589607173</v>
       </c>
       <c r="E4" t="n">
-        <v>9.934229467524872</v>
+        <v>9.948809181108142</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -3440,18 +4139,33 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>6310.4453125</v>
+        <v>8.750119980416409</v>
       </c>
       <c r="L4" t="n">
+        <v>18970.56390677858</v>
+      </c>
+      <c r="M4" t="n">
         <v>482</v>
       </c>
-      <c r="M4" t="n">
-        <v>26.85295877659575</v>
-      </c>
       <c r="N4" t="n">
-        <v>0</v>
+        <v>726.4408961426168</v>
       </c>
       <c r="O4" t="n">
+        <v>2521.839079220629</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.9283850757250121</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>704.662802315798</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.03723455310815493</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3460,16 +4174,16 @@
         <v>43542</v>
       </c>
       <c r="B5" t="n">
-        <v>5047.505108199734</v>
+        <v>5075.901583431952</v>
       </c>
       <c r="C5" t="n">
-        <v>4693.815211330224</v>
+        <v>4676.422714975894</v>
       </c>
       <c r="D5" t="n">
-        <v>73.17196566715555</v>
+        <v>73.10025559768019</v>
       </c>
       <c r="E5" t="n">
-        <v>9.745126579417573</v>
+        <v>9.759706293000843</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -3493,18 +4207,33 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>6827.4296875</v>
+        <v>8.828850012148134</v>
       </c>
       <c r="L5" t="n">
+        <v>18705.69085990358</v>
+      </c>
+      <c r="M5" t="n">
         <v>496</v>
       </c>
-      <c r="M5" t="n">
-        <v>28.44762369791667</v>
-      </c>
       <c r="N5" t="n">
-        <v>0</v>
+        <v>743.7315200387704</v>
       </c>
       <c r="O5" t="n">
+        <v>2557.215444325311</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.9212989316079395</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>713.4370245766494</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.03678687505061722</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3513,16 +4242,16 @@
         <v>43542</v>
       </c>
       <c r="B6" t="n">
-        <v>5160.277854040633</v>
+        <v>5153.230956281038</v>
       </c>
       <c r="C6" t="n">
-        <v>4673.842291054225</v>
+        <v>4655.189799018186</v>
       </c>
       <c r="D6" t="n">
-        <v>74.0928235354023</v>
+        <v>73.98511767222345</v>
       </c>
       <c r="E6" t="n">
-        <v>9.731983671859004</v>
+        <v>9.757217541082161</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -3546,18 +4275,33 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>2746.048828125</v>
+        <v>7.918282461010106</v>
       </c>
       <c r="L6" t="n">
+        <v>13965.56939705456</v>
+      </c>
+      <c r="M6" t="n">
         <v>167</v>
       </c>
-      <c r="M6" t="n">
-        <v>11.68531416223404</v>
-      </c>
       <c r="N6" t="n">
-        <v>0</v>
+        <v>829.5893070855228</v>
       </c>
       <c r="O6" t="n">
+        <v>2084.239476733719</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.9033536104782286</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>721.8888879304465</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.03369481898302173</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>